<commit_message>
Added Mutex lock target for protection for mutating classes
</commit_message>
<xml_diff>
--- a/Cephei.XL/Bond1.xlsx
+++ b/Cephei.XL/Bond1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\source\repos\Cephei2\Cephei.XL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE193A81-0AC6-4DB4-B75D-EEF14787E51D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9725F6F9-81C8-4B1E-AB37-36537A22119F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1287AFFA-50F8-48B2-8168-E284DC333339}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21000" xr2:uid="{1287AFFA-50F8-48B2-8168-E284DC333339}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
   <si>
     <t>calendar</t>
   </si>
@@ -301,9 +301,6 @@
     <t>bondDiscountingTermStructure</t>
   </si>
   <si>
-    <t>bondEngine</t>
-  </si>
-  <si>
     <t>NPV</t>
   </si>
   <si>
@@ -329,6 +326,15 @@
   </si>
   <si>
     <t>+settlementDate</t>
+  </si>
+  <si>
+    <t>bondEnginez</t>
+  </si>
+  <si>
+    <t>bondEnginefi</t>
+  </si>
+  <si>
+    <t>bondEnginefl</t>
   </si>
 </sst>
 </file>
@@ -552,21 +558,57 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>FloatingNPV</v>
+        <v>marketQuotes4</v>
         <stp/>
-        <stp>FloatingNPV</stp>
-        <stp>588410313</stp>
-        <tr r="D56" s="1"/>
+        <stp>marketQuotes4</stp>
+        <stp>0</stp>
+        <tr r="K18" s="1"/>
       </tp>
       <tp t="s">
-        <v>s2y</v>
+        <v>FixedSettlementDatte</v>
         <stp/>
-        <stp>s2y</stp>
-        <stp>2119925512</stp>
-        <tr r="H28" s="1"/>
+        <stp>FixedSettlementDatte</stp>
+        <stp>-798541351</stp>
+        <tr r="B33" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>Semiannual</v>
+        <stp/>
+        <stp>Semiannual</stp>
+        <stp>1704154923</stp>
+        <tr r="E39" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>marketQuotes1</v>
+        <stp/>
+        <stp>marketQuotes1</stp>
+        <stp>0</stp>
+        <tr r="K15" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>marketQuotes0</v>
+        <stp/>
+        <stp>marketQuotes0</stp>
+        <stp>0</stp>
+        <tr r="K14" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>zc1y</v>
+        <stp/>
+        <stp>zc1y</stp>
+        <stp>-2050528296</stp>
+        <tr r="H10" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>couponRate0</v>
         <stp/>
@@ -575,7 +617,7 @@
         <tr r="J14" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>marketQuotes3</v>
         <stp/>
@@ -584,26 +626,14 @@
         <tr r="K17" s="1"/>
       </tp>
       <tp t="s">
-        <v>d1y</v>
+        <v>+settlementDate</v>
         <stp/>
-        <stp>d1y</stp>
-        <stp>2119925464</stp>
-        <tr r="H27" s="1"/>
+        <stp>+settlementDate</stp>
+        <stp>-569911532</stp>
+        <tr r="B3" s="1"/>
       </tp>
-      <tp t="s">
-        <v>s3y</v>
-        <stp/>
-        <stp>s3y</stp>
-        <stp>2119925496</stp>
-        <tr r="H29" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>s5y</v>
-        <stp/>
-        <stp>s5y</stp>
-        <stp>2119925400</stp>
-        <tr r="H30" s="1"/>
-      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>marketQuotes2</v>
         <stp/>
@@ -611,89 +641,44 @@
         <stp>0</stp>
         <tr r="K16" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>FixedRateBond</v>
+        <v>floatcouponpricer2</v>
         <stp/>
-        <stp>FixedRateBond</stp>
-        <stp>-1992100456</stp>
-        <tr r="B37" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>todaysDateSer</v>
-        <stp/>
-        <stp>todaysDateSer</stp>
-        <stp>-1204259704</stp>
-        <tr r="C8" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>marketQuotes1</v>
-        <stp/>
-        <stp>marketQuotes1</stp>
-        <stp>0</stp>
-        <tr r="K15" s="1"/>
+        <stp>floatcouponpricer2</stp>
+        <stp>1878722209</stp>
+        <tr r="B51" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>marketQuotes0</v>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>0.56211286639560409</v>
         <stp/>
-        <stp>marketQuotes0</stp>
-        <stp>0</stp>
-        <tr r="K14" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>s10yratehelpers</v>
+        <stp>FloatingFixedZeroAccruedcoupon</stp>
         <stp/>
-        <stp>s10yratehelpers</stp>
-        <stp>154939048</stp>
-        <tr r="K31" s="1"/>
+        <tr r="D67" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>zc1y</v>
+        <v>FixedZeroPreviouscoupon</v>
         <stp/>
-        <stp>zc1y</stp>
-        <stp>-2050528296</stp>
-        <tr r="H10" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>s15yratehelpers</v>
-        <stp/>
-        <stp>s15yratehelpers</stp>
-        <stp>-96719192</stp>
-        <tr r="K32" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>zc3mRate</v>
-        <stp/>
-        <stp>zc3mRate</stp>
-        <stp>0</stp>
-        <tr r="B10" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>zc6mRate</v>
-        <stp/>
-        <stp>zc6mRate</stp>
-        <stp>0</stp>
-        <tr r="B11" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>FixedSettlementDatte</v>
-        <stp/>
-        <stp>FixedSettlementDatte</stp>
-        <stp>-798541351</stp>
-        <tr r="B33" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>marketQuotes4</v>
-        <stp/>
-        <stp>marketQuotes4</stp>
-        <stp>0</stp>
-        <tr r="K18" s="1"/>
+        <stp>FixedZeroPreviouscoupon</stp>
+        <stp>815396861</stp>
+        <tr r="C60" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>d1mratehelpers</v>
+        <stp/>
+        <stp>d1mratehelpers</stp>
+        <stp>-1371787608</stp>
+        <tr r="K23" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>swFloatingLegIndex</v>
         <stp/>
@@ -701,6 +686,79 @@
         <stp>0</stp>
         <tr r="E46" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>86.317292342665496</v>
+        <stp/>
+        <stp>ZeroDirtyPrice</stp>
+        <stp/>
+        <tr r="B66" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>zc3m</v>
+        <stp/>
+        <stp>zc3m</stp>
+        <stp>-1010340904</stp>
+        <tr r="H8" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d9mRate</v>
+        <stp/>
+        <stp>d9mRate</stp>
+        <stp>0</stp>
+        <tr r="J26" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d6mRate</v>
+        <stp/>
+        <stp>d6mRate</stp>
+        <stp>0</stp>
+        <tr r="J25" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d3mRate</v>
+        <stp/>
+        <stp>d3mRate</stp>
+        <stp>0</stp>
+        <tr r="J24" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d1mRate</v>
+        <stp/>
+        <stp>d1mRate</stp>
+        <stp>0</stp>
+        <tr r="J23" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>bondDiscountingTermStructure</v>
+        <stp/>
+        <stp>bondDiscountingTermStructure</stp>
+        <stp>-1358081960</stp>
+        <tr r="B17" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>FloatingFixedZeroAccruedcoupon</v>
+        <stp/>
+        <stp>FloatingFixedZeroAccruedcoupon</stp>
+        <stp>-1208119139</stp>
+        <tr r="D59" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>#no coupon paid at cashflow date 15/08/2013</v>
+        <stp/>
+        <stp>ZeroNextcoupon</stp>
+        <stp>1029105693#</stp>
+        <tr r="B61" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>FixedRateCashflow</v>
         <stp/>
@@ -708,33 +766,696 @@
         <stp>-77321281</stp>
         <tr r="B38" s="1"/>
       </tp>
+      <tp t="s">
+        <v>+settlementDateAdjustedSer</v>
+        <stp/>
+        <stp>+settlementDateAdjustedSer</stp>
+        <stp>-649169906</stp>
+        <tr r="C4" s="1"/>
+      </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>d1w</v>
+        <v>faceAmount</v>
         <stp/>
-        <stp>d1w</stp>
-        <stp>-303078293</stp>
-        <tr r="H22" s="1"/>
+        <stp>faceAmount</stp>
+        <stp>1079574528</stp>
+        <tr r="B24" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>2.8862499999999999E-2</v>
+        <stp/>
+        <stp>FloatingFixedZeroPreviouscoupon</stp>
+        <stp/>
+        <tr r="D68" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>redemption</v>
+        <stp/>
+        <stp>redemption</stp>
+        <stp>1079574528</stp>
+        <tr r="B13" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>bondhelper4</v>
+        <stp/>
+        <stp>bondhelper4</stp>
+        <stp>-1090572417</stp>
+        <tr r="M18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>4.4999999999999998E-2</v>
+        <stp/>
+        <stp>FixedZeroPreviouscoupon</stp>
+        <stp/>
+        <tr r="C68" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>FixedNextcoupon</v>
+        <stp/>
+        <stp>FixedNextcoupon</stp>
+        <stp>815396861</stp>
+        <tr r="C61" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>d1wRate</v>
+        <stp/>
+        <stp>d1wRate</stp>
+        <stp>0</stp>
+        <tr r="J22" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>floatingBondSchedule</v>
+        <stp/>
+        <stp>floatingBondSchedule</stp>
+        <stp>-2089128530</stp>
+        <tr r="B46" s="1"/>
       </tp>
       <tp t="s">
-        <v>bondDiscountingTermStructure</v>
+        <v>ZeroPreviouscoupon</v>
         <stp/>
-        <stp>bondDiscountingTermStructure</stp>
-        <stp>-1358081960</stp>
-        <tr r="B17" s="1"/>
+        <stp>ZeroPreviouscoupon</stp>
+        <stp>1029105693</stp>
+        <tr r="B60" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>s2yratehelpers</v>
+        <stp/>
+        <stp>s2yratehelpers</stp>
+        <stp>-63164760</stp>
+        <tr r="K28" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>zc3m</v>
+        <v>FloatingDirtyPrice</v>
         <stp/>
-        <stp>zc3m</stp>
-        <stp>-1010340904</stp>
-        <tr r="H8" s="1"/>
+        <stp>FloatingDirtyPrice</stp>
+        <stp>588410313</stp>
+        <tr r="D58" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>d1yRate</v>
+        <stp/>
+        <stp>d1yRate</stp>
+        <stp>0</stp>
+        <tr r="J27" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>s5yRate</v>
+        <stp/>
+        <stp>s5yRate</stp>
+        <stp>0</stp>
+        <tr r="J30" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>s2yRate</v>
+        <stp/>
+        <stp>s2yRate</stp>
+        <stp>0</stp>
+        <tr r="J28" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>s3yRate</v>
+        <stp/>
+        <stp>s3yRate</stp>
+        <stp>0</stp>
+        <tr r="J29" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>86.317292342665496</v>
+        <stp/>
+        <stp>ZeroCleanPrice</stp>
+        <stp/>
+        <tr r="B65" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>d3m</v>
+        <stp/>
+        <stp>d3m</stp>
+        <stp>-1226026113</stp>
+        <tr r="H24" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d6m</v>
+        <stp/>
+        <stp>d6m</stp>
+        <stp>-1226026161</stp>
+        <tr r="H25" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d1m</v>
+        <stp/>
+        <stp>d1m</stp>
+        <stp>-1226026145</stp>
+        <tr r="H23" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>FloatingCleanPrice</v>
+        <stp/>
+        <stp>FloatingCleanPrice</stp>
+        <stp>588410313</stp>
+        <tr r="D57" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>bondhelper2</v>
+        <stp/>
+        <stp>bondhelper2</stp>
+        <stp>-1677774977</stp>
+        <tr r="M16" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>FloatSettlementDatte</v>
+        <stp/>
+        <stp>FloatSettlementDatte</stp>
+        <stp>888501985</stp>
+        <tr r="B42" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>d9m</v>
+        <stp/>
+        <stp>d9m</stp>
+        <stp>-1226026273</stp>
+        <tr r="H26" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>zc6m</v>
+        <stp/>
+        <stp>zc6m</stp>
+        <stp>-792237096</stp>
+        <tr r="H9" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>forwardStart</v>
+        <stp/>
+        <stp>forwardStart</stp>
+        <stp>-223693829</stp>
+        <tr r="E47" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>zcBondsDayCounter</v>
+        <stp/>
+        <stp>zcBondsDayCounter</stp>
+        <stp>0</stp>
+        <tr r="B9" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>107.66828913260423</v>
+        <stp/>
+        <stp>FixedNPV</stp>
+        <stp/>
+        <tr r="C64" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>tolerance</v>
+        <stp/>
+        <stp>tolerance</stp>
+        <stp>-1573562951</stp>
+        <tr r="B14" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>FixedCleanPrice</v>
+        <stp/>
+        <stp>FixedCleanPrice</stp>
+        <stp>-77321281</stp>
+        <tr r="C57" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>s10y</v>
+        <stp/>
+        <stp>s10y</stp>
+        <stp>1121190872</stp>
+        <tr r="H31" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>bondInstruments</v>
+        <stp/>
+        <stp>bondInstruments</stp>
+        <stp>1882299273</stp>
+        <tr r="B16" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>depositDayCounter</v>
+        <stp/>
+        <stp>depositDayCounter</stp>
+        <stp>372029375</stp>
+        <tr r="E43" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>s15y</v>
+        <stp/>
+        <stp>s15y</stp>
+        <stp>772304968</stp>
+        <tr r="H32" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>FixedDirtyPrice</v>
+        <stp/>
+        <stp>FixedDirtyPrice</stp>
+        <stp>-77321281</stp>
+        <tr r="C58" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>107.66828913260423</v>
+        <stp/>
+        <stp>FixedDirtyPrice</stp>
+        <stp/>
+        <tr r="C66" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>+settlementDateAdjusted</v>
+        <stp/>
+        <stp>+settlementDateAdjusted</stp>
+        <stp>-544419191</stp>
+        <tr r="B4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>loglinier</v>
+        <stp/>
+        <stp>loglinier</stp>
+        <stp>0</stp>
+        <tr r="E44" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>fixedBondSchedule</v>
+        <stp/>
+        <stp>fixedBondSchedule</stp>
+        <stp>-2089128530</stp>
+        <tr r="B35" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>39709</v>
+        <stp/>
+        <stp>+settlementDateAdjustedSer</stp>
+        <stp/>
+        <tr r="D4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>todaysDate</v>
+        <stp/>
+        <stp>todaysDate</stp>
+        <stp>-111422835</stp>
+        <tr r="B8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>86.317292342665496</v>
+        <stp/>
+        <stp>ZeroNPV</stp>
+        <stp/>
+        <tr r="B64" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>swFixedLegDayCounter</v>
+        <stp/>
+        <stp>swFixedLegDayCounter</stp>
+        <stp>-748456025</stp>
+        <tr r="E45" s="1"/>
+        <tr r="E51" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>FloatRedemption</v>
+        <stp/>
+        <stp>FloatRedemption</stp>
+        <stp>1079574528</stp>
+        <tr r="B41" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>Gearing</v>
+        <stp/>
+        <stp>Gearing</stp>
+        <stp>1072693248</stp>
+        <tr r="B44" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>FixedRedemption</v>
+        <stp/>
+        <stp>FixedRedemption</stp>
+        <stp>1079574528</stp>
+        <tr r="B32" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>FloatingYield</v>
+        <stp/>
+        <stp>FloatingYield</stp>
+        <stp>-712193011</stp>
+        <tr r="D62" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>termStructureDayCounter</v>
+        <stp/>
+        <stp>termStructureDayCounter</stp>
+        <stp>1443485125</stp>
+        <tr r="E41" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>FixedRateBond</v>
+        <stp/>
+        <stp>FixedRateBond</stp>
+        <stp>1820916808</stp>
+        <tr r="B37" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>Fixing1</v>
+        <stp/>
+        <stp>Fixing1</stp>
+        <stp>1755687198</stp>
+        <tr r="J39" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>bondhelper3</v>
+        <stp/>
+        <stp>bondhelper3</stp>
+        <stp>922693503</stp>
+        <tr r="M17" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>ZeroNPV</v>
+        <stp/>
+        <stp>ZeroNPV</stp>
+        <stp>1001970241</stp>
+        <tr r="B56" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>Spreads</v>
+        <stp/>
+        <stp>Spreads</stp>
+        <stp>-308163663</stp>
+        <tr r="B45" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>2.2009365270878184E-2</v>
+        <stp/>
+        <stp>FloatingYield</stp>
+        <stp/>
+        <tr r="D70" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>106.127528263039</v>
+        <stp/>
+        <stp>FixedCleanPrice</stp>
+        <stp/>
+        <tr r="C65" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>fixingDaysNeg</v>
+        <stp/>
+        <stp>fixingDaysNeg</stp>
+        <stp>-3</stp>
+        <tr r="B7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>fixingDays</v>
+        <stp/>
+        <stp>fixingDays</stp>
+        <stp>3</stp>
+        <tr r="B5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>4.4999999999999998E-2</v>
+        <stp/>
+        <stp>FixedNextcoupon</stp>
+        <stp/>
+        <tr r="C69" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>39706</v>
+        <stp/>
+        <stp>todaysDateSer</stp>
+        <stp/>
+        <tr r="D8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>bondEnginefl</v>
+        <stp/>
+        <stp>bondEnginefl</stp>
+        <stp>246307230</stp>
+        <tr r="B22" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>1.5407608695652275</v>
+        <stp/>
+        <stp>FixedZeroAccruedcoupon</stp>
+        <stp/>
+        <tr r="C67" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>ZeroYield</v>
+        <stp/>
+        <stp>ZeroYield</stp>
+        <stp>-1391670259</stp>
+        <tr r="B62" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>bondEnginefi</v>
+        <stp/>
+        <stp>bondEnginefi</stp>
+        <stp>246307230</stp>
+        <tr r="B21" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>FixedRateCoupon</v>
+        <stp/>
+        <stp>FixedRateCoupon</stp>
+        <stp>1325718839</stp>
+        <tr r="B36" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>zeroCouponBond</v>
+        <stp/>
+        <stp>zeroCouponBond</stp>
+        <stp>-762789832</stp>
+        <tr r="B29" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>bondhelper0</v>
+        <stp/>
+        <stp>bondhelper0</stp>
+        <stp>1862217599</stp>
+        <tr r="M14" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>floatcouponpricer</v>
+        <stp/>
+        <stp>floatcouponpricer</stp>
+        <stp>1741592878</stp>
+        <tr r="B48" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>ActualActualBond</v>
+        <stp/>
+        <stp>ActualActualBond</stp>
+        <stp>1506851973</stp>
+        <tr r="E40" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>FixedZeroAccruedcoupon</v>
+        <stp/>
+        <stp>FixedZeroAccruedcoupon</stp>
+        <stp>815396861</stp>
+        <tr r="C59" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>zc1yPeriod</v>
+        <stp/>
+        <stp>zc1yPeriod</stp>
+        <stp>2119925464</stp>
+        <tr r="E10" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>couponRate1</v>
+        <stp/>
+        <stp>couponRate1</stp>
+        <stp>1162275258</stp>
+        <tr r="J15" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>depoSwapInstruments</v>
+        <stp/>
+        <stp>depoSwapInstruments</stp>
+        <stp>-501517731</stp>
+        <tr r="B18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>ZeroIssueDate</v>
+        <stp/>
+        <stp>ZeroIssueDate</stp>
+        <stp>-12167724</stp>
+        <tr r="B28" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>couponRate3</v>
+        <stp/>
+        <stp>couponRate3</stp>
+        <stp>2013949594</stp>
+        <tr r="J17" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>couponRate2</v>
+        <stp/>
+        <stp>couponRate2</stp>
+        <stp>1067450368</stp>
+        <tr r="J16" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>3.6475570816152846E-2</v>
+        <stp/>
+        <stp>FixedYield</stp>
+        <stp/>
+        <tr r="C70" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>s10yRate</v>
+        <stp/>
+        <stp>s10yRate</stp>
+        <stp>0</stp>
+        <tr r="J31" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>s15yRate</v>
+        <stp/>
+        <stp>s15yRate</stp>
+        <stp>0</stp>
+        <tr r="J32" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>zc1yRate</v>
+        <stp/>
+        <stp>zc1yRate</stp>
+        <stp>0</stp>
+        <tr r="B12" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>instruments</v>
         <stp/>
@@ -750,697 +1471,7 @@
         <tr r="M15" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>libor3mPeriod</v>
-        <stp/>
-        <stp>libor3mPeriod</stp>
-        <stp>-1226026113</stp>
-        <tr r="B40" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>couponRate2</v>
-        <stp/>
-        <stp>couponRate2</stp>
-        <stp>1067450368</stp>
-        <tr r="J16" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>depoSwapTermStructure</v>
-        <stp/>
-        <stp>depoSwapTermStructure</stp>
-        <stp>-1492299688</stp>
-        <tr r="B19" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>s10yRate</v>
-        <stp/>
-        <stp>s10yRate</stp>
-        <stp>0</stp>
-        <tr r="J31" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>s15yRate</v>
-        <stp/>
-        <stp>s15yRate</stp>
-        <stp>0</stp>
-        <tr r="J32" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>zc1yRate</v>
-        <stp/>
-        <stp>zc1yRate</stp>
-        <stp>0</stp>
-        <tr r="B12" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>bondhelper4</v>
-        <stp/>
-        <stp>bondhelper4</stp>
-        <stp>-1090572417</stp>
-        <tr r="M18" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp t="s">
-        <v>zeroCouponBond</v>
-        <stp/>
-        <stp>zeroCouponBond</stp>
-        <stp>RT</stp>
-        <tr r="M88" s="1"/>
-        <tr r="M87" s="1"/>
-        <tr r="E88" s="1"/>
-        <tr r="L88" s="1"/>
-        <tr r="I88" s="1"/>
-        <tr r="K88" s="1"/>
-        <tr r="B88" s="1"/>
-        <tr r="O88" s="1"/>
-        <tr r="F88" s="1"/>
-        <tr r="H88" s="1"/>
-        <tr r="E87" s="1"/>
-        <tr r="P87" s="1"/>
-        <tr r="C87" s="1"/>
-        <tr r="N87" s="1"/>
-        <tr r="N88" s="1"/>
-        <tr r="L87" s="1"/>
-        <tr r="Q87" s="1"/>
-        <tr r="J87" s="1"/>
-        <tr r="B87" s="1"/>
-        <tr r="D88" s="1"/>
-        <tr r="P88" s="1"/>
-        <tr r="F87" s="1"/>
-        <tr r="A87" s="1"/>
-        <tr r="G88" s="1"/>
-        <tr r="I87" s="1"/>
-        <tr r="J88" s="1"/>
-        <tr r="C88" s="1"/>
-        <tr r="O87" s="1"/>
-        <tr r="G87" s="1"/>
-        <tr r="Q88" s="1"/>
-        <tr r="A88" s="1"/>
-        <tr r="K87" s="1"/>
-        <tr r="D87" s="1"/>
-        <tr r="H87" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>couponRate3</v>
-        <stp/>
-        <stp>couponRate3</stp>
-        <stp>2013949594</stp>
-        <tr r="J17" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>2.8862499999999996E-2</v>
-        <stp/>
-        <stp>FloatingFixedZeroPreviouscoupon</stp>
-        <stp/>
-        <tr r="D68" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>floatingBondSchedule</v>
-        <stp/>
-        <stp>floatingBondSchedule</stp>
-        <stp>-2089128530</stp>
-        <tr r="B46" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>depoSwapInstruments</v>
-        <stp/>
-        <stp>depoSwapInstruments</stp>
-        <stp>-501517731</stp>
-        <tr r="B18" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>s2yratehelpers</v>
-        <stp/>
-        <stp>s2yratehelpers</stp>
-        <stp>-63164760</stp>
-        <tr r="K28" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>couponRate1</v>
-        <stp/>
-        <stp>couponRate1</stp>
-        <stp>1162275258</stp>
-        <tr r="J15" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>3.6475570816152846E-2</v>
-        <stp/>
-        <stp>FixedYield</stp>
-        <stp/>
-        <tr r="C70" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>4.4999999999999998E-2</v>
-        <stp/>
-        <stp>FixedZeroPreviouscoupon</stp>
-        <stp/>
-        <tr r="C68" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>bondhelper0</v>
-        <stp/>
-        <stp>bondhelper0</stp>
-        <stp>1862217599</stp>
-        <tr r="M14" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>bondhelper2</v>
-        <stp/>
-        <stp>bondhelper2</stp>
-        <stp>-1677774977</stp>
-        <tr r="M16" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>couponRate4</v>
-        <stp/>
-        <stp>couponRate4</stp>
-        <stp>1325718839</stp>
-        <tr r="J18" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>zc1yPeriod</v>
-        <stp/>
-        <stp>zc1yPeriod</stp>
-        <stp>2119925464</stp>
-        <tr r="E10" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d9m</v>
-        <stp/>
-        <stp>d9m</stp>
-        <stp>-1226026273</stp>
-        <tr r="H26" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>d6m</v>
-        <stp/>
-        <stp>d6m</stp>
-        <stp>-1226026161</stp>
-        <tr r="H25" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d3m</v>
-        <stp/>
-        <stp>d3m</stp>
-        <stp>-1226026113</stp>
-        <tr r="H24" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d1m</v>
-        <stp/>
-        <stp>d1m</stp>
-        <stp>-1226026145</stp>
-        <tr r="H23" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>calendar</v>
-        <stp/>
-        <stp>calendar</stp>
-        <stp>0</stp>
-        <tr r="B2" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>discount</v>
-        <stp/>
-        <stp>discount</stp>
-        <stp>0</stp>
-        <tr r="E42" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>FloatingDirtyPrice</v>
-        <stp/>
-        <stp>FloatingDirtyPrice</stp>
-        <stp>588410313</stp>
-        <tr r="D58" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>FloatingCleanPrice</v>
-        <stp/>
-        <stp>FloatingCleanPrice</stp>
-        <stp>588410313</stp>
-        <tr r="D57" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>FixedYield</v>
-        <stp/>
-        <stp>FixedYield</stp>
-        <stp>-1293104115</stp>
-        <tr r="C62" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d6mratehelpers</v>
-        <stp/>
-        <stp>d6mratehelpers</stp>
-        <stp>-449040728</stp>
-        <tr r="K25" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>zc3mPeriod</v>
-        <stp/>
-        <stp>zc3mPeriod</stp>
-        <stp>-1226026113</stp>
-        <tr r="E8" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>zc6mPeriod</v>
-        <stp/>
-        <stp>zc6mPeriod</stp>
-        <stp>-1226026161</stp>
-        <tr r="E9" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>loglinier</v>
-        <stp/>
-        <stp>loglinier</stp>
-        <stp>0</stp>
-        <tr r="E44" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>d9mratehelpers</v>
-        <stp/>
-        <stp>d9mratehelpers</stp>
-        <stp>-969134424</stp>
-        <tr r="K26" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ZeroSettlementDate</v>
-        <stp/>
-        <stp>ZeroSettlementDate</stp>
-        <stp>-1699218839</stp>
-        <tr r="B27" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>107.10617626620862</v>
-        <stp/>
-        <stp>FloatingCleanPrice</stp>
-        <stp/>
-        <tr r="D65" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>s10y</v>
-        <stp/>
-        <stp>s10y</stp>
-        <stp>1121190872</stp>
-        <tr r="H31" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>depositDayCounter</v>
-        <stp/>
-        <stp>depositDayCounter</stp>
-        <stp>372029375</stp>
-        <tr r="E43" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>floatingRateBondFixedRateBondzeroCouponBondCashflow</v>
-        <stp/>
-        <stp>floatingRateBondFixedRateBondzeroCouponBondCashflow</stp>
-        <stp>588410313</stp>
-        <tr r="D63" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>86.317292342665496</v>
-        <stp/>
-        <stp>ZeroNPV</stp>
-        <stp/>
-        <tr r="B64" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>zc6m</v>
-        <stp/>
-        <stp>zc6m</stp>
-        <stp>-792237096</stp>
-        <tr r="H9" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>forwardStart</v>
-        <stp/>
-        <stp>forwardStart</stp>
-        <stp>-223693829</stp>
-        <tr r="E47" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>zcBondsDayCounter</v>
-        <stp/>
-        <stp>zcBondsDayCounter</stp>
-        <stp>0</stp>
-        <tr r="B9" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#no coupon paid at cashflow date 15/08/2013 ,Bond.nextCouponRate</v>
-        <stp/>
-        <stp>ZeroNextcoupon</stp>
-        <stp>1029105693</stp>
-        <tr r="B61" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ZeroDirtyPrice</v>
-        <stp/>
-        <stp>ZeroDirtyPrice</stp>
-        <stp>1001970241</stp>
-        <tr r="B58" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>102.3205245054389</v>
-        <stp/>
-        <stp>FixedDirtyPrice</stp>
-        <stp/>
-        <tr r="C66" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>3.4298412186850417E-2</v>
-        <stp/>
-        <stp>FloatingNextcoupon</stp>
-        <stp/>
-        <tr r="D69" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>bondEngine</v>
-        <stp/>
-        <stp>bondEngine</stp>
-        <stp>246307230</stp>
-        <tr r="B20" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>FloatingYield</v>
-        <stp/>
-        <stp>FloatingYield</stp>
-        <stp>-712193011</stp>
-        <tr r="D62" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d3mratehelpers</v>
-        <stp/>
-        <stp>d3mratehelpers</stp>
-        <stp>1144794792</stp>
-        <tr r="K24" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>swFixedLegDayCounter</v>
-        <stp/>
-        <stp>swFixedLegDayCounter</stp>
-        <stp>-748456025</stp>
-        <tr r="E51" s="1"/>
-        <tr r="E45" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>FixedRateBondzeroCouponBondCashflow</v>
-        <stp/>
-        <stp>FixedRateBondzeroCouponBondCashflow</stp>
-        <stp>-77321281</stp>
-        <tr r="C63" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>ZeroCleanPrice</v>
-        <stp/>
-        <stp>ZeroCleanPrice</stp>
-        <stp>1001970241</stp>
-        <tr r="B57" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>2.201069345427796E-2</v>
-        <stp/>
-        <stp>FloatingYield</stp>
-        <stp/>
-        <tr r="D70" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>d1yratehelpers</v>
-        <stp/>
-        <stp>d1yratehelpers</stp>
-        <stp>-499372376</stp>
-        <tr r="K27" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>FloatingNextcoupon</v>
-        <stp/>
-        <stp>FloatingNextcoupon</stp>
-        <stp>-1208119139</stp>
-        <tr r="D61" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>107.66828913260423</v>
-        <stp/>
-        <stp>FloatingDirtyPrice</stp>
-        <stp/>
-        <tr r="D66" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>fixingDays</v>
-        <stp/>
-        <stp>fixingDays</stp>
-        <stp>3</stp>
-        <tr r="B5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>zeroCouponBondCashflow</v>
-        <stp/>
-        <stp>zeroCouponBondCashflow</stp>
-        <stp>1001970241</stp>
-        <tr r="B63" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>fixingDaysNeg</v>
-        <stp/>
-        <stp>fixingDaysNeg</stp>
-        <stp>-3</stp>
-        <tr r="B7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>d1wratehelpers</v>
-        <stp/>
-        <stp>d1wratehelpers</stp>
-        <stp>1144794792</stp>
-        <tr r="K22" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>RemptionAmount</v>
-        <stp/>
-        <stp>RemptionAmount</stp>
-        <stp>1079574528</stp>
-        <tr r="B25" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>USDLibor</v>
-        <stp/>
-        <stp>USDLibor</stp>
-        <stp>172051658</stp>
-        <tr r="J37" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>0</v>
-        <stp/>
-        <stp>ZeroPreviouscoupon</stp>
-        <stp/>
-        <tr r="B68" s="1"/>
-      </tp>
-      <tp>
-        <v>100.77866082195537</v>
-        <stp/>
-        <stp>FixedCleanPrice</stp>
-        <stp/>
-        <tr r="C65" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>ConstantOptionletVolatility</v>
-        <stp/>
-        <stp>ConstantOptionletVolatility</stp>
-        <stp>315382730</stp>
-        <tr r="B50" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>optionletvolitility</v>
-        <stp/>
-        <stp>optionletvolitility</stp>
-        <stp>0</stp>
-        <tr r="B49" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>4.4999999999999998E-2</v>
-        <stp/>
-        <stp>FixedNextcoupon</stp>
-        <stp/>
-        <tr r="C69" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>FixedNPV</v>
-        <stp/>
-        <stp>FixedNPV</stp>
-        <stp>-77321281</stp>
-        <tr r="C56" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>s3yratehelpers</v>
-        <stp/>
-        <stp>s3yratehelpers</stp>
-        <stp>-751030616</stp>
-        <tr r="K29" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>s5yratehelpers</v>
-        <stp/>
-        <stp>s5yratehelpers</stp>
-        <stp>1362898600</stp>
-        <tr r="K30" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>39706</v>
-        <stp/>
-        <stp>todaysDateSer</stp>
-        <stp/>
-        <tr r="D8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>d1yRate</v>
-        <stp/>
-        <stp>d1yRate</stp>
-        <stp>0</stp>
-        <tr r="J27" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>s5yRate</v>
-        <stp/>
-        <stp>s5yRate</stp>
-        <stp>0</stp>
-        <tr r="J30" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>s3yRate</v>
-        <stp/>
-        <stp>s3yRate</stp>
-        <stp>0</stp>
-        <tr r="J29" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>s2yRate</v>
-        <stp/>
-        <stp>s2yRate</stp>
-        <stp>0</stp>
-        <tr r="J28" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>ZeroIssueDate</v>
-        <stp/>
-        <stp>ZeroIssueDate</stp>
-        <stp>-12167724</stp>
-        <tr r="B28" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>FixedZeroAccruedcoupon</v>
-        <stp/>
-        <stp>FixedZeroAccruedcoupon</stp>
-        <stp>815396861</stp>
-        <tr r="C59" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>zeroCouponBond</v>
-        <stp/>
-        <stp>zeroCouponBond</stp>
-        <stp>582632856</stp>
-        <tr r="B29" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>floatcouponpricer</v>
-        <stp/>
-        <stp>floatcouponpricer</stp>
-        <stp>1741592878</stp>
-        <tr r="B48" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
       <tp>
         <v>102.3194216915206</v>
         <stp/>
@@ -1449,47 +1480,31 @@
         <tr r="D64" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>ActualActualBond</v>
+        <v>depoSwapTermStructure</v>
         <stp/>
-        <stp>ActualActualBond</stp>
-        <stp>1506851973</stp>
-        <tr r="E40" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>FloatSettlementDatte</v>
-        <stp/>
-        <stp>FloatSettlementDatte</stp>
-        <stp>888501985</stp>
-        <tr r="B42" s="1"/>
+        <stp>depoSwapTermStructure</stp>
+        <stp>-1492299688</stp>
+        <tr r="B19" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>redemption</v>
+        <v>libor3mPeriod</v>
         <stp/>
-        <stp>redemption</stp>
-        <stp>1079574528</stp>
-        <tr r="B13" s="1"/>
+        <stp>libor3mPeriod</stp>
+        <stp>-1226026113</stp>
+        <tr r="B40" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>86.317292342665496</v>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>discount</v>
         <stp/>
-        <stp>ZeroCleanPrice</stp>
-        <stp/>
-        <tr r="B65" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>FixedNextcoupon</v>
-        <stp/>
-        <stp>FixedNextcoupon</stp>
-        <stp>815396861</stp>
-        <tr r="C61" s="1"/>
+        <stp>discount</stp>
+        <stp>0</stp>
+        <tr r="E42" s="1"/>
       </tp>
       <tp t="s">
         <v>settlementDays</v>
@@ -1498,106 +1513,82 @@
         <stp>3</stp>
         <tr r="B6" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>ZeroPreviouscoupon</v>
+        <v>calendar</v>
         <stp/>
-        <stp>ZeroPreviouscoupon</stp>
-        <stp>1029105693</stp>
-        <tr r="B60" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d1wRate</v>
-        <stp/>
-        <stp>d1wRate</stp>
+        <stp>calendar</stp>
         <stp>0</stp>
-        <tr r="J22" s="1"/>
+        <tr r="B2" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>couponRate4</v>
+        <stp/>
+        <stp>couponRate4</stp>
+        <stp>1325718839</stp>
+        <tr r="J18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>floatingRateBond</v>
         <stp/>
         <stp>floatingRateBond</stp>
-        <stp>-544951848</stp>
+        <stp>-922790952</stp>
         <tr r="B47" s="1"/>
       </tp>
-      <tp t="s">
-        <v>FixedZeroPreviouscoupon</v>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>0</v>
         <stp/>
-        <stp>FixedZeroPreviouscoupon</stp>
-        <stp>815396861</stp>
-        <tr r="C60" s="1"/>
+        <stp>ZeroAccruedcoupon</stp>
+        <stp/>
+        <tr r="B67" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>floatcouponpricer2</v>
+        <v>zc3mRate</v>
         <stp/>
-        <stp>floatcouponpricer2</stp>
-        <stp>1878722209</stp>
-        <tr r="B51" s="1"/>
+        <stp>zc3mRate</stp>
+        <stp>0</stp>
+        <tr r="B10" s="1"/>
       </tp>
       <tp t="s">
-        <v>+settlementDate</v>
+        <v>zc6mRate</v>
         <stp/>
-        <stp>+settlementDate</stp>
-        <stp>-569911532</stp>
-        <tr r="B3" s="1"/>
+        <stp>zc6mRate</stp>
+        <stp>0</stp>
+        <tr r="B11" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>d9mRate</v>
+        <v>Quarterly</v>
         <stp/>
-        <stp>d9mRate</stp>
-        <stp>0</stp>
-        <tr r="J26" s="1"/>
+        <stp>Quarterly</stp>
+        <stp>-302169631</stp>
+        <tr r="E49" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>schedule3</v>
+        <stp/>
+        <stp>schedule3</stp>
+        <stp>1913417000</stp>
+        <tr r="L17" s="1"/>
       </tp>
       <tp t="s">
-        <v>d6mRate</v>
+        <v>schedule2</v>
         <stp/>
-        <stp>d6mRate</stp>
-        <stp>0</stp>
-        <tr r="J25" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d1mRate</v>
-        <stp/>
-        <stp>d1mRate</stp>
-        <stp>0</stp>
-        <tr r="J23" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d3mRate</v>
-        <stp/>
-        <stp>d3mRate</stp>
-        <stp>0</stp>
-        <tr r="J24" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>+settlementDateAdjustedSer</v>
-        <stp/>
-        <stp>+settlementDateAdjustedSer</stp>
-        <stp>-649169906</stp>
-        <tr r="C4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>faceAmount</v>
-        <stp/>
-        <stp>faceAmount</stp>
-        <stp>1079574528</stp>
-        <tr r="B24" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>schedule4</v>
-        <stp/>
-        <stp>schedule4</stp>
+        <stp>schedule2</stp>
         <stp>1913417000</stp>
-        <tr r="L18" s="1"/>
+        <tr r="L16" s="1"/>
       </tp>
       <tp t="s">
         <v>schedule1</v>
@@ -1614,93 +1605,57 @@
         <tr r="L14" s="1"/>
       </tp>
       <tp t="s">
-        <v>schedule3</v>
+        <v>schedule4</v>
         <stp/>
-        <stp>schedule3</stp>
+        <stp>schedule4</stp>
         <stp>1913417000</stp>
-        <tr r="L17" s="1"/>
+        <tr r="L18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>d1y</v>
+        <stp/>
+        <stp>d1y</stp>
+        <stp>2119925464</stp>
+        <tr r="H27" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>s3y</v>
+        <stp/>
+        <stp>s3y</stp>
+        <stp>2119925496</stp>
+        <tr r="H29" s="1"/>
       </tp>
       <tp t="s">
-        <v>schedule2</v>
+        <v>s5y</v>
         <stp/>
-        <stp>schedule2</stp>
-        <stp>1913417000</stp>
-        <tr r="L16" s="1"/>
+        <stp>s5y</stp>
+        <stp>2119925400</stp>
+        <tr r="H30" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>0</v>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>s2y</v>
         <stp/>
-        <stp>ZeroAccruedcoupon</stp>
-        <stp/>
-        <tr r="B67" s="1"/>
+        <stp>s2y</stp>
+        <stp>2119925512</stp>
+        <tr r="H28" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>Quarterly</v>
+        <v>todaysDateSer</v>
         <stp/>
-        <stp>Quarterly</stp>
-        <stp>-302169631</stp>
-        <tr r="E49" s="1"/>
+        <stp>todaysDateSer</stp>
+        <stp>-1204259704</stp>
+        <tr r="C8" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>Semiannual</v>
-        <stp/>
-        <stp>Semiannual</stp>
-        <stp>1704154923</stp>
-        <tr r="E39" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>0.56211286639560409</v>
-        <stp/>
-        <stp>FloatingFixedZeroAccruedcoupon</stp>
-        <stp/>
-        <tr r="D67" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>FloatingFixedZeroAccruedcoupon</v>
-        <stp/>
-        <stp>FloatingFixedZeroAccruedcoupon</stp>
-        <stp>-1208119139</stp>
-        <tr r="D59" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>#no coupon paid at cashflow date 15/08/2013 ,Bond.nextCouponRate</v>
-        <stp/>
-        <stp>ZeroNextcoupon</stp>
-        <stp>1029105693/</stp>
-        <tr r="B61" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>ZeroAccruedcoupon</v>
-        <stp/>
-        <stp>ZeroAccruedcoupon</stp>
-        <stp>1029105693</stp>
-        <tr r="B59" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>86.317292342665496</v>
-        <stp/>
-        <stp>ZeroDirtyPrice</stp>
-        <stp/>
-        <tr r="B66" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
       <tp>
         <v>3.0000642156600955E-2</v>
         <stp/>
@@ -1709,53 +1664,77 @@
         <tr r="B70" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>d1mratehelpers</v>
+        <v>ZeroAccruedcoupon</v>
         <stp/>
-        <stp>d1mratehelpers</stp>
-        <stp>-1371787608</stp>
-        <tr r="K23" s="1"/>
+        <stp>ZeroAccruedcoupon</stp>
+        <stp>1029105693</stp>
+        <tr r="B59" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>FloatingNPV</v>
+        <stp/>
+        <stp>FloatingNPV</stp>
+        <stp>588410313</stp>
+        <tr r="D56" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>Spreads</v>
+        <v>d1w</v>
         <stp/>
-        <stp>Spreads</stp>
-        <stp>-308163663</stp>
-        <tr r="B45" s="1"/>
+        <stp>d1w</stp>
+        <stp>-303078293</stp>
+        <tr r="H22" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>Actual365Fixed</v>
+        <v>s10yratehelpers</v>
         <stp/>
-        <stp>Actual365Fixed</stp>
+        <stp>s10yratehelpers</stp>
+        <stp>154939048</stp>
+        <tr r="K31" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>s15yratehelpers</v>
+        <stp/>
+        <stp>s15yratehelpers</stp>
+        <stp>-96719192</stp>
+        <tr r="K32" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>ConstantOptionletVolatility</v>
+        <stp/>
+        <stp>ConstantOptionletVolatility</stp>
+        <stp>315382730</stp>
+        <tr r="B50" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>USDLibor</v>
+        <stp/>
+        <stp>USDLibor</stp>
+        <stp>172051658</stp>
+        <tr r="J37" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>optionletvolitility</v>
+        <stp/>
+        <stp>optionletvolitility</stp>
         <stp>0</stp>
-        <tr r="E50" s="1"/>
+        <tr r="B49" s="1"/>
       </tp>
-      <tp t="s">
-        <v>ZeroNPV</v>
-        <stp/>
-        <stp>ZeroNPV</stp>
-        <stp>1001970241</stp>
-        <tr r="B56" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ZeroYield</v>
-        <stp/>
-        <stp>ZeroYield</stp>
-        <stp>-1391670259</stp>
-        <tr r="B62" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>Fixing1</v>
-        <stp/>
-        <stp>Fixing1</stp>
-        <stp>1755687198</stp>
-        <tr r="J39" s="1"/>
-      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>actual360</v>
         <stp/>
@@ -1764,93 +1743,61 @@
         <tr r="E48" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>termStructureDayCounter</v>
+        <v>s3yratehelpers</v>
         <stp/>
-        <stp>termStructureDayCounter</stp>
-        <stp>1443485125</stp>
-        <tr r="E41" s="1"/>
+        <stp>s3yratehelpers</stp>
+        <stp>-751030616</stp>
+        <tr r="K29" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp t="s">
-        <v>FixedRateBondzeroCouponBondCashflow</v>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>102.3194216915206</v>
         <stp/>
-        <stp>FixedRateBondzeroCouponBondCashflow</stp>
-        <stp>CT</stp>
-        <tr r="H50" s="1"/>
-        <tr r="I59" s="1"/>
-        <tr r="H59" s="1"/>
-        <tr r="I60" s="1"/>
-        <tr r="I56" s="1"/>
-        <tr r="I45" s="1"/>
-        <tr r="H44" s="1"/>
-        <tr r="I49" s="1"/>
-        <tr r="H45" s="1"/>
-        <tr r="H54" s="1"/>
-        <tr r="I48" s="1"/>
-        <tr r="I54" s="1"/>
-        <tr r="H48" s="1"/>
-        <tr r="H42" s="1"/>
-        <tr r="H61" s="1"/>
-        <tr r="H52" s="1"/>
-        <tr r="I57" s="1"/>
-        <tr r="H57" s="1"/>
-        <tr r="I51" s="1"/>
-        <tr r="I55" s="1"/>
-        <tr r="I53" s="1"/>
-        <tr r="H51" s="1"/>
-        <tr r="I46" s="1"/>
-        <tr r="I63" s="1"/>
-        <tr r="I52" s="1"/>
-        <tr r="H46" s="1"/>
-        <tr r="I50" s="1"/>
-        <tr r="I43" s="1"/>
-        <tr r="H63" s="1"/>
-        <tr r="H53" s="1"/>
-        <tr r="H49" s="1"/>
-        <tr r="H62" s="1"/>
-        <tr r="H60" s="1"/>
-        <tr r="H58" s="1"/>
-        <tr r="I44" s="1"/>
-        <tr r="I61" s="1"/>
-        <tr r="H55" s="1"/>
-        <tr r="H47" s="1"/>
-        <tr r="H56" s="1"/>
-        <tr r="H43" s="1"/>
-        <tr r="I62" s="1"/>
-        <tr r="I47" s="1"/>
-        <tr r="I42" s="1"/>
-        <tr r="I58" s="1"/>
+        <stp>FloatingDirtyPrice</stp>
+        <stp/>
+        <tr r="D66" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>FixedRateCoupon</v>
+        <v>FloatingNextcoupon</v>
         <stp/>
-        <stp>FixedRateCoupon</stp>
-        <stp>1325718839</stp>
-        <tr r="B36" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>bondhelper3</v>
-        <stp/>
-        <stp>bondhelper3</stp>
-        <stp>922693503</stp>
-        <tr r="M17" s="1"/>
+        <stp>FloatingNextcoupon</stp>
+        <stp>-1208119139</stp>
+        <tr r="D61" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>1.5407608695652275</v>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>s5yratehelpers</v>
         <stp/>
-        <stp>FixedZeroAccruedcoupon</stp>
-        <stp/>
-        <tr r="C67" s="1"/>
+        <stp>s5yratehelpers</stp>
+        <stp>1362898600</stp>
+        <tr r="K30" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>Actual365Fixed</v>
+        <stp/>
+        <stp>Actual365Fixed</stp>
+        <stp>0</stp>
+        <tr r="E50" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>ZeroPreviouscoupon</stp>
+        <stp/>
+        <tr r="B68" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>FixedIssueDate</v>
         <stp/>
@@ -1859,53 +1806,93 @@
         <tr r="B34" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>FixedRateBond</v>
+        <v>ZeroCleanPrice</v>
         <stp/>
-        <stp>FixedRateBond</stp>
-        <stp>RT</stp>
-        <tr r="C90" s="1"/>
-        <tr r="M90" s="1"/>
-        <tr r="E89" s="1"/>
-        <tr r="P89" s="1"/>
-        <tr r="Q90" s="1"/>
-        <tr r="R90" s="1"/>
-        <tr r="D90" s="1"/>
-        <tr r="S90" s="1"/>
-        <tr r="R89" s="1"/>
-        <tr r="H90" s="1"/>
-        <tr r="N89" s="1"/>
-        <tr r="G89" s="1"/>
-        <tr r="L89" s="1"/>
-        <tr r="J89" s="1"/>
-        <tr r="Q89" s="1"/>
-        <tr r="K89" s="1"/>
-        <tr r="B90" s="1"/>
-        <tr r="B89" s="1"/>
-        <tr r="O89" s="1"/>
-        <tr r="A90" s="1"/>
-        <tr r="E90" s="1"/>
-        <tr r="O90" s="1"/>
-        <tr r="A89" s="1"/>
-        <tr r="L90" s="1"/>
-        <tr r="K90" s="1"/>
-        <tr r="D89" s="1"/>
-        <tr r="S89" s="1"/>
-        <tr r="M89" s="1"/>
-        <tr r="N90" s="1"/>
-        <tr r="G90" s="1"/>
-        <tr r="C89" s="1"/>
-        <tr r="J90" s="1"/>
-        <tr r="H89" s="1"/>
-        <tr r="I90" s="1"/>
-        <tr r="I89" s="1"/>
-        <tr r="P90" s="1"/>
-        <tr r="F89" s="1"/>
-        <tr r="F90" s="1"/>
+        <stp>ZeroCleanPrice</stp>
+        <stp>1001970241</stp>
+        <tr r="B57" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d1yratehelpers</v>
+        <stp/>
+        <stp>d1yratehelpers</stp>
+        <stp>-499372376</stp>
+        <tr r="K27" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>FixedRateBondzeroCouponBondCashflow</v>
+        <stp/>
+        <stp>FixedRateBondzeroCouponBondCashflow</stp>
+        <stp>-77321281</stp>
+        <tr r="C63" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>zeroCouponBondCashflow</v>
+        <stp/>
+        <stp>zeroCouponBondCashflow</stp>
+        <stp>1001970241</stp>
+        <tr r="B63" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp t="s">
+        <v>FixedRateBondzeroCouponBondCashflow</v>
+        <stp/>
+        <stp>FixedRateBondzeroCouponBondCashflow</stp>
+        <stp>CT</stp>
+        <tr r="I56" s="1"/>
+        <tr r="H63" s="1"/>
+        <tr r="I60" s="1"/>
+        <tr r="H58" s="1"/>
+        <tr r="H47" s="1"/>
+        <tr r="H49" s="1"/>
+        <tr r="I46" s="1"/>
+        <tr r="H56" s="1"/>
+        <tr r="H61" s="1"/>
+        <tr r="H46" s="1"/>
+        <tr r="I52" s="1"/>
+        <tr r="I62" s="1"/>
+        <tr r="H60" s="1"/>
+        <tr r="H44" s="1"/>
+        <tr r="I58" s="1"/>
+        <tr r="H48" s="1"/>
+        <tr r="I55" s="1"/>
+        <tr r="H57" s="1"/>
+        <tr r="H45" s="1"/>
+        <tr r="I42" s="1"/>
+        <tr r="H54" s="1"/>
+        <tr r="H50" s="1"/>
+        <tr r="I44" s="1"/>
+        <tr r="I59" s="1"/>
+        <tr r="H62" s="1"/>
+        <tr r="I47" s="1"/>
+        <tr r="H52" s="1"/>
+        <tr r="H42" s="1"/>
+        <tr r="I57" s="1"/>
+        <tr r="I61" s="1"/>
+        <tr r="I51" s="1"/>
+        <tr r="H53" s="1"/>
+        <tr r="H43" s="1"/>
+        <tr r="I63" s="1"/>
+        <tr r="I45" s="1"/>
+        <tr r="I50" s="1"/>
+        <tr r="H59" s="1"/>
+        <tr r="I53" s="1"/>
+        <tr r="H51" s="1"/>
+        <tr r="H55" s="1"/>
+        <tr r="I49" s="1"/>
+        <tr r="I54" s="1"/>
+        <tr r="I48" s="1"/>
+        <tr r="I43" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>FloatIssueDate</v>
         <stp/>
@@ -1914,28 +1901,34 @@
         <tr r="B43" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>USgovi</v>
+        <v>FixedNPV</v>
         <stp/>
-        <stp>USgovi</stp>
-        <stp>814714544</stp>
-        <tr r="E38" s="1"/>
+        <stp>FixedNPV</stp>
+        <stp>-77321281</stp>
+        <tr r="C56" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>+settlementDateAdjusted</v>
+        <v>RemptionAmount</v>
         <stp/>
-        <stp>+settlementDateAdjusted</stp>
-        <stp>-544419191</stp>
-        <tr r="B4" s="1"/>
+        <stp>RemptionAmount</stp>
+        <stp>1079574528</stp>
+        <tr r="B25" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>s15y</v>
+        <v>d1wratehelpers</v>
         <stp/>
-        <stp>s15y</stp>
-        <stp>772304968</stp>
-        <tr r="H32" s="1"/>
+        <stp>d1wratehelpers</stp>
+        <stp>1144794792</stp>
+        <tr r="K22" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>USDLibor1</v>
         <stp/>
@@ -1944,55 +1937,165 @@
         <tr r="J39" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>bondInstruments</v>
+        <v>USgovi</v>
         <stp/>
-        <stp>bondInstruments</stp>
-        <stp>1882299273</stp>
-        <tr r="B16" s="1"/>
+        <stp>USgovi</stp>
+        <stp>814714544</stp>
+        <tr r="E38" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>39709</v>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>bondEnginez</v>
         <stp/>
-        <stp>+settlementDateAdjustedSer</stp>
-        <stp/>
-        <tr r="D4" s="1"/>
+        <stp>bondEnginez</stp>
+        <stp>246307230</stp>
+        <tr r="B20" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>FixedCleanPrice</v>
+        <v>ZeroSettlementDate</v>
         <stp/>
-        <stp>FixedCleanPrice</stp>
-        <stp>-77321281</stp>
-        <tr r="C57" s="1"/>
+        <stp>ZeroSettlementDate</stp>
+        <stp>-1699218839</stp>
+        <tr r="B27" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>tolerance</v>
+        <v>d3mratehelpers</v>
         <stp/>
-        <stp>tolerance</stp>
-        <stp>-1573562951</stp>
-        <tr r="B14" s="1"/>
+        <stp>d3mratehelpers</stp>
+        <stp>1144794792</stp>
+        <tr r="K24" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>101.75730882512499</v>
+        <stp/>
+        <stp>FloatingCleanPrice</stp>
+        <stp/>
+        <tr r="D65" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>zc6mPeriod</v>
+        <stp/>
+        <stp>zc6mPeriod</stp>
+        <stp>-1226026161</stp>
+        <tr r="E9" s="1"/>
       </tp>
       <tp t="s">
-        <v>FixedRedemption</v>
+        <v>zc3mPeriod</v>
         <stp/>
-        <stp>FixedRedemption</stp>
-        <stp>1079574528</stp>
-        <tr r="B32" s="1"/>
+        <stp>zc3mPeriod</stp>
+        <stp>-1226026113</stp>
+        <tr r="E8" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>Gearing</v>
+        <v>FixedYield</v>
         <stp/>
-        <stp>Gearing</stp>
-        <stp>1072693248</stp>
-        <tr r="B44" s="1"/>
+        <stp>FixedYield</stp>
+        <stp>-1293104115</stp>
+        <tr r="C62" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp>
+        <v>3.4298412186850417E-2</v>
+        <stp/>
+        <stp>FloatingNextcoupon</stp>
+        <stp/>
+        <tr r="D69" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>d6mratehelpers</v>
+        <stp/>
+        <stp>d6mratehelpers</stp>
+        <stp>-449040728</stp>
+        <tr r="K25" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>d9mratehelpers</v>
+        <stp/>
+        <stp>d9mratehelpers</stp>
+        <stp>-969134424</stp>
+        <tr r="K26" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+      <tp t="s">
+        <v>floatingRateBondFixedRateBondzeroCouponBondCashflow</v>
+        <stp/>
+        <stp>floatingRateBondFixedRateBondzeroCouponBondCashflow</stp>
+        <stp>CT</stp>
+        <tr r="H78" s="1"/>
+        <tr r="H70" s="1"/>
+        <tr r="I72" s="1"/>
+        <tr r="I74" s="1"/>
+        <tr r="I78" s="1"/>
+        <tr r="I67" s="1"/>
+        <tr r="H82" s="1"/>
+        <tr r="H84" s="1"/>
+        <tr r="I83" s="1"/>
+        <tr r="H74" s="1"/>
+        <tr r="H72" s="1"/>
+        <tr r="I64" s="1"/>
+        <tr r="H69" s="1"/>
+        <tr r="H85" s="1"/>
+        <tr r="I69" s="1"/>
+        <tr r="H83" s="1"/>
+        <tr r="H77" s="1"/>
+        <tr r="I85" s="1"/>
+        <tr r="H67" s="1"/>
+        <tr r="H68" s="1"/>
+        <tr r="I70" s="1"/>
+        <tr r="I77" s="1"/>
+        <tr r="I75" s="1"/>
+        <tr r="H64" s="1"/>
+        <tr r="H71" s="1"/>
+        <tr r="H75" s="1"/>
+        <tr r="I82" s="1"/>
+        <tr r="I84" s="1"/>
+        <tr r="H66" s="1"/>
+        <tr r="I65" s="1"/>
+        <tr r="H80" s="1"/>
+        <tr r="H73" s="1"/>
+        <tr r="I66" s="1"/>
+        <tr r="I81" s="1"/>
+        <tr r="I76" s="1"/>
+        <tr r="H81" s="1"/>
+        <tr r="I73" s="1"/>
+        <tr r="H76" s="1"/>
+        <tr r="I79" s="1"/>
+        <tr r="I80" s="1"/>
+        <tr r="H79" s="1"/>
+        <tr r="H65" s="1"/>
+        <tr r="I71" s="1"/>
+        <tr r="I68" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+      <tp t="s">
+        <v>floatingRateBondFixedRateBondzeroCouponBondCashflow</v>
+        <stp/>
+        <stp>floatingRateBondFixedRateBondzeroCouponBondCashflow</stp>
+        <stp>588410313</stp>
+        <tr r="D63" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>FloatingFixedZeroPreviouscoupon</v>
         <stp/>
@@ -2001,101 +2104,13 @@
         <tr r="D60" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
+    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
-        <v>fixedBondSchedule</v>
+        <v>ZeroDirtyPrice</v>
         <stp/>
-        <stp>fixedBondSchedule</stp>
-        <stp>-2089128530</stp>
-        <tr r="B35" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>FloatRedemption</v>
-        <stp/>
-        <stp>FloatRedemption</stp>
-        <stp>1079574528</stp>
-        <tr r="B41" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp>
-        <v>107.66828913260423</v>
-        <stp/>
-        <stp>FixedNPV</stp>
-        <stp/>
-        <tr r="C64" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>FixedDirtyPrice</v>
-        <stp/>
-        <stp>FixedDirtyPrice</stp>
-        <stp>-77321281</stp>
-        <tr r="C58" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f053909ac93b4ea9bf4b7bdd96ace956">
-      <tp t="s">
-        <v>floatingRateBondFixedRateBondzeroCouponBondCashflow</v>
-        <stp/>
-        <stp>floatingRateBondFixedRateBondzeroCouponBondCashflow</stp>
-        <stp>CT</stp>
-        <tr r="H85" s="1"/>
-        <tr r="I74" s="1"/>
-        <tr r="I79" s="1"/>
-        <tr r="I83" s="1"/>
-        <tr r="H68" s="1"/>
-        <tr r="I72" s="1"/>
-        <tr r="H81" s="1"/>
-        <tr r="I77" s="1"/>
-        <tr r="H67" s="1"/>
-        <tr r="H72" s="1"/>
-        <tr r="I67" s="1"/>
-        <tr r="H69" s="1"/>
-        <tr r="I80" s="1"/>
-        <tr r="H66" s="1"/>
-        <tr r="H77" s="1"/>
-        <tr r="I64" s="1"/>
-        <tr r="I85" s="1"/>
-        <tr r="I70" s="1"/>
-        <tr r="H65" s="1"/>
-        <tr r="H70" s="1"/>
-        <tr r="I71" s="1"/>
-        <tr r="I65" s="1"/>
-        <tr r="H79" s="1"/>
-        <tr r="I84" s="1"/>
-        <tr r="H82" s="1"/>
-        <tr r="I81" s="1"/>
-        <tr r="H78" s="1"/>
-        <tr r="H84" s="1"/>
-        <tr r="I76" s="1"/>
-        <tr r="H73" s="1"/>
-        <tr r="H80" s="1"/>
-        <tr r="I66" s="1"/>
-        <tr r="I68" s="1"/>
-        <tr r="H71" s="1"/>
-        <tr r="I75" s="1"/>
-        <tr r="H83" s="1"/>
-        <tr r="H74" s="1"/>
-        <tr r="H76" s="1"/>
-        <tr r="I73" s="1"/>
-        <tr r="I82" s="1"/>
-        <tr r="H64" s="1"/>
-        <tr r="I78" s="1"/>
-        <tr r="I69" s="1"/>
-        <tr r="H75" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.4879f5bf3e2748c6967a46182b26b7f2">
-      <tp t="s">
-        <v>todaysDate</v>
-        <stp/>
-        <stp>todaysDate</stp>
-        <stp>-111422835</stp>
-        <tr r="B8" s="1"/>
+        <stp>ZeroDirtyPrice</stp>
+        <stp>1001970241</stp>
+        <tr r="B58" s="1"/>
       </tp>
     </main>
   </volType>
@@ -2435,10 +2450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28025E14-2DBA-4FA2-A060-A0CB22BD8F4F}">
-  <dimension ref="A1:S90"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2489,7 +2504,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="str">
         <f>+_xll._Date1(A3,C3)</f>
@@ -2971,14 +2986,21 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B20" t="str">
-        <f>+_xll._DiscountingBondEngine(A20,B17,TRUE,$B$4)</f>
-        <v>bondEngine</v>
+        <f>+_xll._DiscountingBondEngine(A20,$B$17,TRUE,$B$4)</f>
+        <v>bondEnginez</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" t="str">
+        <f>+_xll._DiscountingBondEngine(A21,$B$17,TRUE,$B$4)</f>
+        <v>bondEnginefi</v>
+      </c>
       <c r="E21" s="12" t="s">
         <v>23</v>
       </c>
@@ -3002,6 +3024,13 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" t="str">
+        <f>+_xll._DiscountingBondEngine(A22,$B$17,TRUE,$B$4)</f>
+        <v>bondEnginefl</v>
+      </c>
       <c r="E22" s="7" t="s">
         <v>24</v>
       </c>
@@ -3400,7 +3429,7 @@
         <v>56</v>
       </c>
       <c r="B37" t="str">
-        <f>+_xll._FixedRateBond(A37,B6,B24,B35,B36,E40,"ModifiedFollowing",B32,B34,B2,,,,,B20,B8)</f>
+        <f>+_xll._FixedRateBond(A37,B6,B24,B35,B36,E40,"ModifiedFollowing",B32,B34,B2,,,,,B21,B8)</f>
         <v>FixedRateBond</v>
       </c>
       <c r="E37" t="s">
@@ -3416,7 +3445,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" t="str">
         <f>+_xll._Bond_cashflows(A38,B37)</f>
@@ -3601,7 +3630,7 @@
         <v>71</v>
       </c>
       <c r="B47" t="str">
-        <f>+_xll._FloatingRateBond2(A47,B6,B24,B46,J39,E48,"ModifiedFollowing",2,+B44,B45,,,TRUE,B41,B43,B20,B51,B8)</f>
+        <f>+_xll._FloatingRateBond2(A47,B6,B24,B46,J39,E48,"ModifiedFollowing",2,+B44,B45,,,TRUE,B41,B43,B22,B51,B8)</f>
         <v>floatingRateBond</v>
       </c>
       <c r="E47" t="str">
@@ -3734,7 +3763,7 @@
         <v>76</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C55" t="s">
         <v>82</v>
@@ -3752,7 +3781,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B56" t="str">
         <f>+_xll._Instrument_NPV(B$55&amp;$A56,B54)</f>
@@ -3871,7 +3900,7 @@
       </c>
       <c r="B61" t="str">
         <f>+_xll._Bond_nextCouponRate(B$55&amp;$A61,B54)</f>
-        <v>#no coupon paid at cashflow date 15/08/2013 ,Bond.nextCouponRate</v>
+        <v>#no coupon paid at cashflow date 15/08/2013</v>
       </c>
       <c r="C61" t="str">
         <f>+_xll._Bond_nextCouponRate(C$55&amp;$A61,C54)</f>
@@ -3890,7 +3919,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B62" t="str">
         <f>+_xll._Bond_yield(B$55&amp;$A62,B54,$E$48,"Compounded","Annual")</f>
@@ -3913,7 +3942,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B63" t="str">
         <f>+_xll._Bond_cashflows(B54&amp;A$63,B54)</f>
@@ -3928,7 +3957,7 @@
         <v>floatingRateBondFixedRateBondzeroCouponBondCashflow</v>
       </c>
       <c r="F63" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H63">
         <v>100</v>
@@ -3973,11 +4002,11 @@
       </c>
       <c r="C65">
         <f>+_xll._Value(C57)</f>
-        <v>100.77866082195537</v>
+        <v>106.127528263039</v>
       </c>
       <c r="D65">
         <f>+_xll._Value(D57)</f>
-        <v>107.10617626620862</v>
+        <v>101.75730882512499</v>
       </c>
       <c r="H65" t="str">
         <v>#NA</v>
@@ -3997,11 +4026,11 @@
       </c>
       <c r="C66">
         <f>+_xll._Value(C58)</f>
-        <v>102.3205245054389</v>
+        <v>107.66828913260423</v>
       </c>
       <c r="D66">
         <f>+_xll._Value(D58)</f>
-        <v>107.66828913260423</v>
+        <v>102.3194216915206</v>
       </c>
       <c r="H66" t="str">
         <v>#NA</v>
@@ -4049,7 +4078,7 @@
       </c>
       <c r="D68">
         <f>+_xll._Value(D60)</f>
-        <v>2.8862499999999996E-2</v>
+        <v>2.8862499999999999E-2</v>
       </c>
       <c r="H68" t="str">
         <v>#NA</v>
@@ -4097,7 +4126,7 @@
       </c>
       <c r="D70">
         <f>+_xll._Value(D62)</f>
-        <v>2.201069345427796E-2</v>
+        <v>2.2009365270878184E-2</v>
       </c>
       <c r="H70" t="str">
         <v>#NA</v>
@@ -4108,7 +4137,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B71" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H71" t="str">
         <v>#NA</v>
@@ -4189,7 +4218,7 @@
         <v>40107</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="81" spans="7:9" x14ac:dyDescent="0.35">
       <c r="H81">
         <v>0.65014134434928483</v>
       </c>
@@ -4197,7 +4226,7 @@
         <v>40199</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="82" spans="7:9" x14ac:dyDescent="0.35">
       <c r="H82">
         <v>0.63602853580461316</v>
       </c>
@@ -4205,7 +4234,7 @@
         <v>40289</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="83" spans="7:9" x14ac:dyDescent="0.35">
       <c r="H83">
         <v>0.73560473983753116</v>
       </c>
@@ -4213,7 +4242,7 @@
         <v>40380</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="84" spans="7:9" x14ac:dyDescent="0.35">
       <c r="H84">
         <v>0.92793509955574272</v>
       </c>
@@ -4221,241 +4250,15 @@
         <v>40472</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="85" spans="7:9" x14ac:dyDescent="0.35">
       <c r="G85" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H85">
         <v>100</v>
       </c>
       <c r="I85" s="1">
         <v>40472</v>
-      </c>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A87" t="e">
-        <f t="array" ref="A87:Q88">+_xll._Value_Range(B54,"RT")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="F87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="G87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="M87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="N87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="O87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P87" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q87" t="e">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="B88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="F88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="G88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="M88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="N88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="O88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P88" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q88" t="e">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A89" t="e">
-        <f t="array" ref="A89:S90">+_xll._Value_Range(C54,"RT")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="F89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="G89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="M89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="N89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="O89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="R89" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="S89" t="e">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="B90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="E90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="F90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="G90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="I90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="M90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="N90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="O90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="R90" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="S90" t="e">
-        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added additional spin locking
</commit_message>
<xml_diff>
--- a/Cephei.XL/Bond1.xlsx
+++ b/Cephei.XL/Bond1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\source\repos\Cephei2\Cephei.XL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9725F6F9-81C8-4B1E-AB37-36537A22119F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0284BD8-A35D-4364-8F53-4583EE87BAF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21000" xr2:uid="{1287AFFA-50F8-48B2-8168-E284DC333339}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1287AFFA-50F8-48B2-8168-E284DC333339}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -558,23 +558,14 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>marketQuotes4</v>
+        <v>zc1y</v>
         <stp/>
-        <stp>marketQuotes4</stp>
-        <stp>0</stp>
-        <tr r="K18" s="1"/>
+        <stp>zc1y</stp>
+        <stp>-2050528296</stp>
+        <tr r="H10" s="1"/>
       </tp>
-      <tp t="s">
-        <v>FixedSettlementDatte</v>
-        <stp/>
-        <stp>FixedSettlementDatte</stp>
-        <stp>-798541351</stp>
-        <tr r="B33" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>Semiannual</v>
         <stp/>
@@ -583,48 +574,7 @@
         <tr r="E39" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>marketQuotes1</v>
-        <stp/>
-        <stp>marketQuotes1</stp>
-        <stp>0</stp>
-        <tr r="K15" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>marketQuotes0</v>
-        <stp/>
-        <stp>marketQuotes0</stp>
-        <stp>0</stp>
-        <tr r="K14" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>zc1y</v>
-        <stp/>
-        <stp>zc1y</stp>
-        <stp>-2050528296</stp>
-        <tr r="H10" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>couponRate0</v>
-        <stp/>
-        <stp>couponRate0</stp>
-        <stp>-1165563463</stp>
-        <tr r="J14" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>marketQuotes3</v>
-        <stp/>
-        <stp>marketQuotes3</stp>
-        <stp>0</stp>
-        <tr r="K17" s="1"/>
-      </tp>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>+settlementDate</v>
         <stp/>
@@ -633,16 +583,50 @@
         <tr r="B3" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>marketQuotes2</v>
+        <v>d1mratehelpers</v>
         <stp/>
-        <stp>marketQuotes2</stp>
-        <stp>0</stp>
-        <tr r="K16" s="1"/>
+        <stp>d1mratehelpers</stp>
+        <stp>-1371787608</stp>
+        <tr r="K23" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>floatingRateBond</v>
+        <stp/>
+        <stp>floatingRateBond</stp>
+        <stp>-922790952</stp>
+        <tr r="B47" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>bondDiscountingTermStructure</v>
+        <stp/>
+        <stp>bondDiscountingTermStructure</stp>
+        <stp>-1358081960</stp>
+        <tr r="B17" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>zc3m</v>
+        <stp/>
+        <stp>zc3m</stp>
+        <stp>-1010340904</stp>
+        <tr r="H8" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>FixedZeroPreviouscoupon</v>
+        <stp/>
+        <stp>FixedZeroPreviouscoupon</stp>
+        <stp>815396861</stp>
+        <tr r="C60" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>floatcouponpricer2</v>
         <stp/>
@@ -651,34 +635,21 @@
         <tr r="B51" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>0.56211286639560409</v>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>+settlementDateAdjustedSer</v>
         <stp/>
-        <stp>FloatingFixedZeroAccruedcoupon</stp>
+        <stp>+settlementDateAdjustedSer</stp>
+        <stp>-649169906</stp>
+        <tr r="C4" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>faceAmount</v>
         <stp/>
-        <tr r="D67" s="1"/>
+        <stp>faceAmount</stp>
+        <stp>1079574528</stp>
+        <tr r="B24" s="1"/>
       </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>FixedZeroPreviouscoupon</v>
-        <stp/>
-        <stp>FixedZeroPreviouscoupon</stp>
-        <stp>815396861</stp>
-        <tr r="C60" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>d1mratehelpers</v>
-        <stp/>
-        <stp>d1mratehelpers</stp>
-        <stp>-1371787608</stp>
-        <tr r="K23" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>swFloatingLegIndex</v>
         <stp/>
@@ -687,23 +658,7 @@
         <tr r="E46" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>86.317292342665496</v>
-        <stp/>
-        <stp>ZeroDirtyPrice</stp>
-        <stp/>
-        <tr r="B66" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>zc3m</v>
-        <stp/>
-        <stp>zc3m</stp>
-        <stp>-1010340904</stp>
-        <tr r="H8" s="1"/>
-      </tp>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>d9mRate</v>
         <stp/>
@@ -712,11 +667,11 @@
         <tr r="J26" s="1"/>
       </tp>
       <tp t="s">
-        <v>d6mRate</v>
+        <v>d1mRate</v>
         <stp/>
-        <stp>d6mRate</stp>
+        <stp>d1mRate</stp>
         <stp>0</stp>
-        <tr r="J25" s="1"/>
+        <tr r="J23" s="1"/>
       </tp>
       <tp t="s">
         <v>d3mRate</v>
@@ -726,21 +681,23 @@
         <tr r="J24" s="1"/>
       </tp>
       <tp t="s">
-        <v>d1mRate</v>
+        <v>d6mRate</v>
         <stp/>
-        <stp>d1mRate</stp>
+        <stp>d6mRate</stp>
         <stp>0</stp>
-        <tr r="J23" s="1"/>
+        <tr r="J25" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>bondDiscountingTermStructure</v>
+        <v>ZeroNextcoupon</v>
         <stp/>
-        <stp>bondDiscountingTermStructure</stp>
-        <stp>-1358081960</stp>
-        <tr r="B17" s="1"/>
+        <stp>ZeroNextcoupon</stp>
+        <stp>1029105693#</stp>
+        <tr r="B61" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>FloatingFixedZeroAccruedcoupon</v>
         <stp/>
@@ -749,95 +706,7 @@
         <tr r="D59" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>#no coupon paid at cashflow date 15/08/2013</v>
-        <stp/>
-        <stp>ZeroNextcoupon</stp>
-        <stp>1029105693#</stp>
-        <tr r="B61" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>FixedRateCashflow</v>
-        <stp/>
-        <stp>FixedRateCashflow</stp>
-        <stp>-77321281</stp>
-        <tr r="B38" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>+settlementDateAdjustedSer</v>
-        <stp/>
-        <stp>+settlementDateAdjustedSer</stp>
-        <stp>-649169906</stp>
-        <tr r="C4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>faceAmount</v>
-        <stp/>
-        <stp>faceAmount</stp>
-        <stp>1079574528</stp>
-        <tr r="B24" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>2.8862499999999999E-2</v>
-        <stp/>
-        <stp>FloatingFixedZeroPreviouscoupon</stp>
-        <stp/>
-        <tr r="D68" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>redemption</v>
-        <stp/>
-        <stp>redemption</stp>
-        <stp>1079574528</stp>
-        <tr r="B13" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>bondhelper4</v>
-        <stp/>
-        <stp>bondhelper4</stp>
-        <stp>-1090572417</stp>
-        <tr r="M18" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>4.4999999999999998E-2</v>
-        <stp/>
-        <stp>FixedZeroPreviouscoupon</stp>
-        <stp/>
-        <tr r="C68" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>FixedNextcoupon</v>
-        <stp/>
-        <stp>FixedNextcoupon</stp>
-        <stp>815396861</stp>
-        <tr r="C61" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>d1wRate</v>
-        <stp/>
-        <stp>d1wRate</stp>
-        <stp>0</stp>
-        <tr r="J22" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>floatingBondSchedule</v>
         <stp/>
@@ -845,12 +714,14 @@
         <stp>-2089128530</stp>
         <tr r="B46" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>ZeroPreviouscoupon</v>
+        <v>redemption</v>
         <stp/>
-        <stp>ZeroPreviouscoupon</stp>
-        <stp>1029105693</stp>
-        <tr r="B60" s="1"/>
+        <stp>redemption</stp>
+        <stp>1079574528</stp>
+        <tr r="B13" s="1"/>
       </tp>
       <tp t="s">
         <v>s2yratehelpers</v>
@@ -860,22 +731,74 @@
         <tr r="K28" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>FloatingDirtyPrice</v>
+        <v>d1wRate</v>
         <stp/>
-        <stp>FloatingDirtyPrice</stp>
-        <stp>588410313</stp>
-        <tr r="D58" s="1"/>
+        <stp>d1wRate</stp>
+        <stp>0</stp>
+        <tr r="J22" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>3.6475570816152846E-2</v>
+        <stp/>
+        <stp>FixedYield</stp>
+        <stp/>
+        <tr r="C70" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>d1yRate</v>
+        <v>ZeroPreviouscoupon</v>
         <stp/>
-        <stp>d1yRate</stp>
+        <stp>ZeroPreviouscoupon</stp>
+        <stp>1029105693</stp>
+        <tr r="B60" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>FixedNextcoupon</v>
+        <stp/>
+        <stp>FixedNextcoupon</stp>
+        <stp>815396861</stp>
+        <tr r="C61" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>ActualActualBond</v>
+        <stp/>
+        <stp>ActualActualBond</stp>
+        <stp>1506851973</stp>
+        <tr r="E40" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>102.3194216915206</v>
+        <stp/>
+        <stp>FloatingNPV</stp>
+        <stp/>
+        <tr r="D64" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>s3yRate</v>
+        <stp/>
+        <stp>s3yRate</stp>
         <stp>0</stp>
-        <tr r="J27" s="1"/>
+        <tr r="J29" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>s2yRate</v>
+        <stp/>
+        <stp>s2yRate</stp>
+        <stp>0</stp>
+        <tr r="J28" s="1"/>
       </tp>
       <tp t="s">
         <v>s5yRate</v>
@@ -885,43 +808,386 @@
         <tr r="J30" s="1"/>
       </tp>
       <tp t="s">
-        <v>s2yRate</v>
+        <v>d1yRate</v>
         <stp/>
-        <stp>s2yRate</stp>
+        <stp>d1yRate</stp>
         <stp>0</stp>
-        <tr r="J28" s="1"/>
+        <tr r="J27" s="1"/>
       </tp>
       <tp t="s">
-        <v>s3yRate</v>
+        <v>FloatingCleanPrice</v>
         <stp/>
-        <stp>s3yRate</stp>
-        <stp>0</stp>
-        <tr r="J29" s="1"/>
+        <stp>FloatingCleanPrice</stp>
+        <stp>588410313</stp>
+        <tr r="D57" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>86.317292342665496</v>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>ZeroIssueDate</v>
         <stp/>
-        <stp>ZeroCleanPrice</stp>
-        <stp/>
-        <tr r="B65" s="1"/>
+        <stp>ZeroIssueDate</stp>
+        <stp>-12167724</stp>
+        <tr r="B28" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>d3m</v>
+        <v>FloatingDirtyPrice</v>
         <stp/>
-        <stp>d3m</stp>
-        <stp>-1226026113</stp>
-        <tr r="H24" s="1"/>
+        <stp>FloatingDirtyPrice</stp>
+        <stp>588410313</stp>
+        <tr r="D58" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>FloatSettlementDatte</v>
+        <stp/>
+        <stp>FloatSettlementDatte</stp>
+        <stp>888501985</stp>
+        <tr r="B42" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>FixedCleanPrice</v>
+        <stp/>
+        <stp>FixedCleanPrice</stp>
+        <stp>-77321281</stp>
+        <tr r="C57" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>bondInstruments</v>
+        <stp/>
+        <stp>bondInstruments</stp>
+        <stp>1882299273</stp>
+        <tr r="B16" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>tolerance</v>
+        <stp/>
+        <stp>tolerance</stp>
+        <stp>-1573562951</stp>
+        <tr r="B14" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>+settlementDateAdjusted</v>
+        <stp/>
+        <stp>+settlementDateAdjusted</stp>
+        <stp>-544419191</stp>
+        <tr r="B4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>todaysDate</v>
+        <stp/>
+        <stp>todaysDate</stp>
+        <stp>-111422835</stp>
+        <tr r="B8" s="1"/>
       </tp>
       <tp t="s">
-        <v>d6m</v>
+        <v>s15y</v>
         <stp/>
-        <stp>d6m</stp>
-        <stp>-1226026161</stp>
-        <tr r="H25" s="1"/>
+        <stp>s15y</stp>
+        <stp>772304968</stp>
+        <tr r="H32" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>FloatingFixedZeroPreviouscoupon</v>
+        <stp/>
+        <stp>FloatingFixedZeroPreviouscoupon</stp>
+        <stp>-1208119139</stp>
+        <tr r="D60" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>101.75730882512499</v>
+        <stp/>
+        <stp>FloatingCleanPrice</stp>
+        <stp/>
+        <tr r="D65" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>fixedBondSchedule</v>
+        <stp/>
+        <stp>fixedBondSchedule</stp>
+        <stp>-2089128530</stp>
+        <tr r="B35" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>FixedDirtyPrice</v>
+        <stp/>
+        <stp>FixedDirtyPrice</stp>
+        <stp>-77321281</stp>
+        <tr r="C58" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>FloatingYield</v>
+        <stp/>
+        <stp>FloatingYield</stp>
+        <stp>-712193011</stp>
+        <tr r="D62" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>3.4298412186850417E-2</v>
+        <stp/>
+        <stp>FloatingNextcoupon</stp>
+        <stp/>
+        <tr r="D69" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>FloatRedemption</v>
+        <stp/>
+        <stp>FloatRedemption</stp>
+        <stp>1079574528</stp>
+        <tr r="B41" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>Gearing</v>
+        <stp/>
+        <stp>Gearing</stp>
+        <stp>1072693248</stp>
+        <tr r="B44" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>FixedRedemption</v>
+        <stp/>
+        <stp>FixedRedemption</stp>
+        <stp>1079574528</stp>
+        <tr r="B32" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>fixingDays</v>
+        <stp/>
+        <stp>fixingDays</stp>
+        <stp>3</stp>
+        <tr r="B5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>bondhelper3</v>
+        <stp/>
+        <stp>bondhelper3</stp>
+        <stp>922693503</stp>
+        <tr r="M17" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>termStructureDayCounter</v>
+        <stp/>
+        <stp>termStructureDayCounter</stp>
+        <stp>1443485125</stp>
+        <tr r="E41" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>ZeroNPV</v>
+        <stp/>
+        <stp>ZeroNPV</stp>
+        <stp>1001970241</stp>
+        <tr r="B56" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>fixingDaysNeg</v>
+        <stp/>
+        <stp>fixingDaysNeg</stp>
+        <stp>-3</stp>
+        <tr r="B7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>Fixing1</v>
+        <stp/>
+        <stp>Fixing1</stp>
+        <stp>1755687198</stp>
+        <tr r="J39" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>Spreads</v>
+        <stp/>
+        <stp>Spreads</stp>
+        <stp>-308163663</stp>
+        <tr r="B45" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>ZeroPreviouscoupon</stp>
+        <stp/>
+        <tr r="B68" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>102.3194216915206</v>
+        <stp/>
+        <stp>FloatingDirtyPrice</stp>
+        <stp/>
+        <tr r="D66" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>FixedRateBond</v>
+        <stp/>
+        <stp>FixedRateBond</stp>
+        <stp>1820916808</stp>
+        <tr r="B37" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>39706</v>
+        <stp/>
+        <stp>todaysDateSer</stp>
+        <stp/>
+        <tr r="D8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>2.2009365270878184E-2</v>
+        <stp/>
+        <stp>FloatingYield</stp>
+        <stp/>
+        <tr r="D70" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>bondEnginefl</v>
+        <stp/>
+        <stp>bondEnginefl</stp>
+        <stp>246307230</stp>
+        <tr r="B22" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>actual360</v>
+        <stp/>
+        <stp>actual360</stp>
+        <stp>372029375</stp>
+        <tr r="E48" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>FixedRateCoupon</v>
+        <stp/>
+        <stp>FixedRateCoupon</stp>
+        <stp>1325718839</stp>
+        <tr r="B36" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>bondEnginefi</v>
+        <stp/>
+        <stp>bondEnginefi</stp>
+        <stp>246307230</stp>
+        <tr r="B21" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>ZeroYield</v>
+        <stp/>
+        <stp>ZeroYield</stp>
+        <stp>-1391670259</stp>
+        <tr r="B62" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>bondhelper0</v>
+        <stp/>
+        <stp>bondhelper0</stp>
+        <stp>1862217599</stp>
+        <tr r="M14" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>depoSwapInstruments</v>
+        <stp/>
+        <stp>depoSwapInstruments</stp>
+        <stp>-501517731</stp>
+        <tr r="B18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp t="s">
+        <v>#no coupon paid at cashflow date 15/08/2013 ,Bond.nextCouponRate</v>
+        <stp/>
+        <stp>ZeroNextcoupon</stp>
+        <stp/>
+        <tr r="B69" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>zc1yPeriod</v>
+        <stp/>
+        <stp>zc1yPeriod</stp>
+        <stp>2119925464</stp>
+        <tr r="E10" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>zeroCouponBond</v>
+        <stp/>
+        <stp>zeroCouponBond</stp>
+        <stp>-762789832</stp>
+        <tr r="B29" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>couponRate1</v>
+        <stp/>
+        <stp>couponRate1</stp>
+        <stp>1162275258</stp>
+        <tr r="J15" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>couponRate3</v>
+        <stp/>
+        <stp>couponRate3</stp>
+        <stp>2013949594</stp>
+        <tr r="J17" s="1"/>
       </tp>
       <tp t="s">
         <v>d1m</v>
@@ -931,16 +1197,57 @@
         <tr r="H23" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>FloatingCleanPrice</v>
+        <v>d6m</v>
         <stp/>
-        <stp>FloatingCleanPrice</stp>
-        <stp>588410313</stp>
-        <tr r="D57" s="1"/>
+        <stp>d6m</stp>
+        <stp>-1226026161</stp>
+        <tr r="H25" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>d3m</v>
+        <stp/>
+        <stp>d3m</stp>
+        <stp>-1226026113</stp>
+        <tr r="H24" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>d9m</v>
+        <stp/>
+        <stp>d9m</stp>
+        <stp>-1226026273</stp>
+        <tr r="H26" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>bondhelper1</v>
+        <stp/>
+        <stp>bondhelper1</stp>
+        <stp>-738250881</stp>
+        <tr r="M15" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>instruments</v>
+        <stp/>
+        <stp>instruments</stp>
+        <stp>-192993751</stp>
+        <tr r="B15" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>FixedZeroAccruedcoupon</v>
+        <stp/>
+        <stp>FixedZeroAccruedcoupon</stp>
+        <stp>815396861</stp>
+        <tr r="C59" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>bondhelper2</v>
         <stp/>
@@ -949,488 +1256,14 @@
         <tr r="M16" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>FloatSettlementDatte</v>
+        <v>zc1yRate</v>
         <stp/>
-        <stp>FloatSettlementDatte</stp>
-        <stp>888501985</stp>
-        <tr r="B42" s="1"/>
+        <stp>zc1yRate</stp>
+        <stp>0</stp>
+        <tr r="B12" s="1"/>
       </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>d9m</v>
-        <stp/>
-        <stp>d9m</stp>
-        <stp>-1226026273</stp>
-        <tr r="H26" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>zc6m</v>
-        <stp/>
-        <stp>zc6m</stp>
-        <stp>-792237096</stp>
-        <tr r="H9" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>forwardStart</v>
-        <stp/>
-        <stp>forwardStart</stp>
-        <stp>-223693829</stp>
-        <tr r="E47" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>zcBondsDayCounter</v>
-        <stp/>
-        <stp>zcBondsDayCounter</stp>
-        <stp>0</stp>
-        <tr r="B9" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>107.66828913260423</v>
-        <stp/>
-        <stp>FixedNPV</stp>
-        <stp/>
-        <tr r="C64" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>tolerance</v>
-        <stp/>
-        <stp>tolerance</stp>
-        <stp>-1573562951</stp>
-        <tr r="B14" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>FixedCleanPrice</v>
-        <stp/>
-        <stp>FixedCleanPrice</stp>
-        <stp>-77321281</stp>
-        <tr r="C57" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>s10y</v>
-        <stp/>
-        <stp>s10y</stp>
-        <stp>1121190872</stp>
-        <tr r="H31" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>bondInstruments</v>
-        <stp/>
-        <stp>bondInstruments</stp>
-        <stp>1882299273</stp>
-        <tr r="B16" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>depositDayCounter</v>
-        <stp/>
-        <stp>depositDayCounter</stp>
-        <stp>372029375</stp>
-        <tr r="E43" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>s15y</v>
-        <stp/>
-        <stp>s15y</stp>
-        <stp>772304968</stp>
-        <tr r="H32" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>FixedDirtyPrice</v>
-        <stp/>
-        <stp>FixedDirtyPrice</stp>
-        <stp>-77321281</stp>
-        <tr r="C58" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>107.66828913260423</v>
-        <stp/>
-        <stp>FixedDirtyPrice</stp>
-        <stp/>
-        <tr r="C66" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>+settlementDateAdjusted</v>
-        <stp/>
-        <stp>+settlementDateAdjusted</stp>
-        <stp>-544419191</stp>
-        <tr r="B4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>loglinier</v>
-        <stp/>
-        <stp>loglinier</stp>
-        <stp>0</stp>
-        <tr r="E44" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>fixedBondSchedule</v>
-        <stp/>
-        <stp>fixedBondSchedule</stp>
-        <stp>-2089128530</stp>
-        <tr r="B35" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>39709</v>
-        <stp/>
-        <stp>+settlementDateAdjustedSer</stp>
-        <stp/>
-        <tr r="D4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>todaysDate</v>
-        <stp/>
-        <stp>todaysDate</stp>
-        <stp>-111422835</stp>
-        <tr r="B8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>86.317292342665496</v>
-        <stp/>
-        <stp>ZeroNPV</stp>
-        <stp/>
-        <tr r="B64" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>swFixedLegDayCounter</v>
-        <stp/>
-        <stp>swFixedLegDayCounter</stp>
-        <stp>-748456025</stp>
-        <tr r="E45" s="1"/>
-        <tr r="E51" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>FloatRedemption</v>
-        <stp/>
-        <stp>FloatRedemption</stp>
-        <stp>1079574528</stp>
-        <tr r="B41" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>Gearing</v>
-        <stp/>
-        <stp>Gearing</stp>
-        <stp>1072693248</stp>
-        <tr r="B44" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>FixedRedemption</v>
-        <stp/>
-        <stp>FixedRedemption</stp>
-        <stp>1079574528</stp>
-        <tr r="B32" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>FloatingYield</v>
-        <stp/>
-        <stp>FloatingYield</stp>
-        <stp>-712193011</stp>
-        <tr r="D62" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>termStructureDayCounter</v>
-        <stp/>
-        <stp>termStructureDayCounter</stp>
-        <stp>1443485125</stp>
-        <tr r="E41" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>FixedRateBond</v>
-        <stp/>
-        <stp>FixedRateBond</stp>
-        <stp>1820916808</stp>
-        <tr r="B37" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>Fixing1</v>
-        <stp/>
-        <stp>Fixing1</stp>
-        <stp>1755687198</stp>
-        <tr r="J39" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>bondhelper3</v>
-        <stp/>
-        <stp>bondhelper3</stp>
-        <stp>922693503</stp>
-        <tr r="M17" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>ZeroNPV</v>
-        <stp/>
-        <stp>ZeroNPV</stp>
-        <stp>1001970241</stp>
-        <tr r="B56" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>Spreads</v>
-        <stp/>
-        <stp>Spreads</stp>
-        <stp>-308163663</stp>
-        <tr r="B45" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>2.2009365270878184E-2</v>
-        <stp/>
-        <stp>FloatingYield</stp>
-        <stp/>
-        <tr r="D70" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>106.127528263039</v>
-        <stp/>
-        <stp>FixedCleanPrice</stp>
-        <stp/>
-        <tr r="C65" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>fixingDaysNeg</v>
-        <stp/>
-        <stp>fixingDaysNeg</stp>
-        <stp>-3</stp>
-        <tr r="B7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>fixingDays</v>
-        <stp/>
-        <stp>fixingDays</stp>
-        <stp>3</stp>
-        <tr r="B5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>4.4999999999999998E-2</v>
-        <stp/>
-        <stp>FixedNextcoupon</stp>
-        <stp/>
-        <tr r="C69" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>39706</v>
-        <stp/>
-        <stp>todaysDateSer</stp>
-        <stp/>
-        <tr r="D8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>bondEnginefl</v>
-        <stp/>
-        <stp>bondEnginefl</stp>
-        <stp>246307230</stp>
-        <tr r="B22" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>1.5407608695652275</v>
-        <stp/>
-        <stp>FixedZeroAccruedcoupon</stp>
-        <stp/>
-        <tr r="C67" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>ZeroYield</v>
-        <stp/>
-        <stp>ZeroYield</stp>
-        <stp>-1391670259</stp>
-        <tr r="B62" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>bondEnginefi</v>
-        <stp/>
-        <stp>bondEnginefi</stp>
-        <stp>246307230</stp>
-        <tr r="B21" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>FixedRateCoupon</v>
-        <stp/>
-        <stp>FixedRateCoupon</stp>
-        <stp>1325718839</stp>
-        <tr r="B36" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>zeroCouponBond</v>
-        <stp/>
-        <stp>zeroCouponBond</stp>
-        <stp>-762789832</stp>
-        <tr r="B29" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>bondhelper0</v>
-        <stp/>
-        <stp>bondhelper0</stp>
-        <stp>1862217599</stp>
-        <tr r="M14" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>floatcouponpricer</v>
-        <stp/>
-        <stp>floatcouponpricer</stp>
-        <stp>1741592878</stp>
-        <tr r="B48" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>ActualActualBond</v>
-        <stp/>
-        <stp>ActualActualBond</stp>
-        <stp>1506851973</stp>
-        <tr r="E40" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>FixedZeroAccruedcoupon</v>
-        <stp/>
-        <stp>FixedZeroAccruedcoupon</stp>
-        <stp>815396861</stp>
-        <tr r="C59" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>zc1yPeriod</v>
-        <stp/>
-        <stp>zc1yPeriod</stp>
-        <stp>2119925464</stp>
-        <tr r="E10" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>couponRate1</v>
-        <stp/>
-        <stp>couponRate1</stp>
-        <stp>1162275258</stp>
-        <tr r="J15" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>depoSwapInstruments</v>
-        <stp/>
-        <stp>depoSwapInstruments</stp>
-        <stp>-501517731</stp>
-        <tr r="B18" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>ZeroIssueDate</v>
-        <stp/>
-        <stp>ZeroIssueDate</stp>
-        <stp>-12167724</stp>
-        <tr r="B28" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>couponRate3</v>
-        <stp/>
-        <stp>couponRate3</stp>
-        <stp>2013949594</stp>
-        <tr r="J17" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>couponRate2</v>
-        <stp/>
-        <stp>couponRate2</stp>
-        <stp>1067450368</stp>
-        <tr r="J16" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>3.6475570816152846E-2</v>
-        <stp/>
-        <stp>FixedYield</stp>
-        <stp/>
-        <tr r="C70" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>s10yRate</v>
         <stp/>
@@ -1446,41 +1279,50 @@
         <tr r="J32" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>zc1yRate</v>
+        <v>floatcouponpricer</v>
         <stp/>
-        <stp>zc1yRate</stp>
-        <stp>0</stp>
-        <tr r="B12" s="1"/>
+        <stp>floatcouponpricer</stp>
+        <stp>1741592878</stp>
+        <tr r="B48" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>couponRate2</v>
+        <stp/>
+        <stp>couponRate2</stp>
+        <stp>1067450368</stp>
+        <tr r="J16" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>instruments</v>
+        <v>libor3mPeriod</v>
         <stp/>
-        <stp>instruments</stp>
-        <stp>-192993751</stp>
-        <tr r="B15" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>bondhelper1</v>
-        <stp/>
-        <stp>bondhelper1</stp>
-        <stp>-738250881</stp>
-        <tr r="M15" s="1"/>
+        <stp>libor3mPeriod</stp>
+        <stp>-1226026113</stp>
+        <tr r="B40" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
       <tp>
-        <v>102.3194216915206</v>
+        <v>4.4999999999999998E-2</v>
         <stp/>
-        <stp>FloatingNPV</stp>
+        <stp>FixedZeroPreviouscoupon</stp>
         <stp/>
-        <tr r="D64" s="1"/>
+        <tr r="C68" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>settlementDays</v>
+        <stp/>
+        <stp>settlementDays</stp>
+        <stp>3</stp>
+        <tr r="B6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>depoSwapTermStructure</v>
         <stp/>
@@ -1489,16 +1331,7 @@
         <tr r="B19" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>libor3mPeriod</v>
-        <stp/>
-        <stp>libor3mPeriod</stp>
-        <stp>-1226026113</stp>
-        <tr r="B40" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>discount</v>
         <stp/>
@@ -1507,15 +1340,6 @@
         <tr r="E42" s="1"/>
       </tp>
       <tp t="s">
-        <v>settlementDays</v>
-        <stp/>
-        <stp>settlementDays</stp>
-        <stp>3</stp>
-        <tr r="B6" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
         <v>calendar</v>
         <stp/>
         <stp>calendar</stp>
@@ -1523,7 +1347,16 @@
         <tr r="B2" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>bondhelper4</v>
+        <stp/>
+        <stp>bondhelper4</stp>
+        <stp>-1090572417</stp>
+        <tr r="M18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>couponRate4</v>
         <stp/>
@@ -1532,25 +1365,62 @@
         <tr r="J18" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>floatingRateBond</v>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>86.317292342665496</v>
         <stp/>
-        <stp>floatingRateBond</stp>
-        <stp>-922790952</stp>
-        <tr r="B47" s="1"/>
+        <stp>ZeroCleanPrice</stp>
+        <stp/>
+        <tr r="B65" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
       <tp>
-        <v>0</v>
+        <v>2.8862499999999999E-2</v>
         <stp/>
-        <stp>ZeroAccruedcoupon</stp>
+        <stp>FloatingFixedZeroPreviouscoupon</stp>
         <stp/>
-        <tr r="B67" s="1"/>
+        <tr r="D68" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>schedule2</v>
+        <stp/>
+        <stp>schedule2</stp>
+        <stp>1913417000</stp>
+        <tr r="L16" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>schedule3</v>
+        <stp/>
+        <stp>schedule3</stp>
+        <stp>1913417000</stp>
+        <tr r="L17" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>schedule0</v>
+        <stp/>
+        <stp>schedule0</stp>
+        <stp>1913417000</stp>
+        <tr r="L14" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>schedule1</v>
+        <stp/>
+        <stp>schedule1</stp>
+        <stp>1913417000</stp>
+        <tr r="L15" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>schedule4</v>
+        <stp/>
+        <stp>schedule4</stp>
+        <stp>1913417000</stp>
+        <tr r="L18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>zc3mRate</v>
         <stp/>
@@ -1565,8 +1435,6 @@
         <stp>0</stp>
         <tr r="B11" s="1"/>
       </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>Quarterly</v>
         <stp/>
@@ -1575,44 +1443,46 @@
         <tr r="E49" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>3.0000642156600955E-2</v>
+        <stp/>
+        <stp>ZeroYield</stp>
+        <stp/>
+        <tr r="B70" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>schedule3</v>
+        <v>s2y</v>
         <stp/>
-        <stp>schedule3</stp>
-        <stp>1913417000</stp>
-        <tr r="L17" s="1"/>
+        <stp>s2y</stp>
+        <stp>2119925512</stp>
+        <tr r="H28" s="1"/>
       </tp>
       <tp t="s">
-        <v>schedule2</v>
+        <v>FixedRateCashflow</v>
         <stp/>
-        <stp>schedule2</stp>
-        <stp>1913417000</stp>
-        <tr r="L16" s="1"/>
+        <stp>FixedRateCashflow</stp>
+        <stp>-77321281</stp>
+        <tr r="B38" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>s5y</v>
+        <stp/>
+        <stp>s5y</stp>
+        <stp>2119925400</stp>
+        <tr r="H30" s="1"/>
       </tp>
       <tp t="s">
-        <v>schedule1</v>
+        <v>s3y</v>
         <stp/>
-        <stp>schedule1</stp>
-        <stp>1913417000</stp>
-        <tr r="L15" s="1"/>
+        <stp>s3y</stp>
+        <stp>2119925496</stp>
+        <tr r="H29" s="1"/>
       </tp>
-      <tp t="s">
-        <v>schedule0</v>
-        <stp/>
-        <stp>schedule0</stp>
-        <stp>1913417000</stp>
-        <tr r="L14" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>schedule4</v>
-        <stp/>
-        <stp>schedule4</stp>
-        <stp>1913417000</stp>
-        <tr r="L18" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
       <tp t="s">
         <v>d1y</v>
         <stp/>
@@ -1621,32 +1491,39 @@
         <tr r="H27" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>s3y</v>
+        <v>FixedSettlementDatte</v>
         <stp/>
-        <stp>s3y</stp>
-        <stp>2119925496</stp>
-        <tr r="H29" s="1"/>
+        <stp>FixedSettlementDatte</stp>
+        <stp>-798541351</stp>
+        <tr r="B33" s="1"/>
       </tp>
       <tp t="s">
-        <v>s5y</v>
+        <v>marketQuotes4</v>
         <stp/>
-        <stp>s5y</stp>
-        <stp>2119925400</stp>
-        <tr r="H30" s="1"/>
+        <stp>marketQuotes4</stp>
+        <stp>0</stp>
+        <tr r="K18" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>s2y</v>
+        <v>s10yratehelpers</v>
         <stp/>
-        <stp>s2y</stp>
-        <stp>2119925512</stp>
-        <tr r="H28" s="1"/>
+        <stp>s10yratehelpers</stp>
+        <stp>154939048</stp>
+        <tr r="K31" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>FloatingNPV</v>
+        <stp/>
+        <stp>FloatingNPV</stp>
+        <stp>588410313</stp>
+        <tr r="D56" s="1"/>
+      </tp>
       <tp t="s">
         <v>todaysDateSer</v>
         <stp/>
@@ -1655,32 +1532,7 @@
         <tr r="C8" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>3.0000642156600955E-2</v>
-        <stp/>
-        <stp>ZeroYield</stp>
-        <stp/>
-        <tr r="B70" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>ZeroAccruedcoupon</v>
-        <stp/>
-        <stp>ZeroAccruedcoupon</stp>
-        <stp>1029105693</stp>
-        <tr r="B59" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>FloatingNPV</v>
-        <stp/>
-        <stp>FloatingNPV</stp>
-        <stp>588410313</stp>
-        <tr r="D56" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>d1w</v>
         <stp/>
@@ -1689,16 +1541,84 @@
         <tr r="H22" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>s10yratehelpers</v>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>0.56211286639560409</v>
         <stp/>
-        <stp>s10yratehelpers</stp>
-        <stp>154939048</stp>
-        <tr r="K31" s="1"/>
+        <stp>FloatingFixedZeroAccruedcoupon</stp>
+        <stp/>
+        <tr r="D67" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>marketQuotes0</v>
+        <stp/>
+        <stp>marketQuotes0</stp>
+        <stp>0</stp>
+        <tr r="K14" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>marketQuotes1</v>
+        <stp/>
+        <stp>marketQuotes1</stp>
+        <stp>0</stp>
+        <tr r="K15" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>marketQuotes2</v>
+        <stp/>
+        <stp>marketQuotes2</stp>
+        <stp>0</stp>
+        <tr r="K16" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>ZeroAccruedcoupon</v>
+        <stp/>
+        <stp>ZeroAccruedcoupon</stp>
+        <stp>1029105693</stp>
+        <tr r="B59" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>86.317292342665496</v>
+        <stp/>
+        <stp>ZeroDirtyPrice</stp>
+        <stp/>
+        <tr r="B66" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>couponRate0</v>
+        <stp/>
+        <stp>couponRate0</stp>
+        <stp>-1165563463</stp>
+        <tr r="J14" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>marketQuotes3</v>
+        <stp/>
+        <stp>marketQuotes3</stp>
+        <stp>0</stp>
+        <tr r="K17" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>ZeroAccruedcoupon</stp>
+        <stp/>
+        <tr r="B67" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>s15yratehelpers</v>
         <stp/>
@@ -1707,7 +1627,86 @@
         <tr r="K32" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>Actual365Fixed</v>
+        <stp/>
+        <stp>Actual365Fixed</stp>
+        <stp>0</stp>
+        <tr r="E50" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>USDLibor</v>
+        <stp/>
+        <stp>USDLibor</stp>
+        <stp>172051658</stp>
+        <tr r="J37" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp t="s">
+        <v>FixedRateBondzeroCouponBondCashflow</v>
+        <stp/>
+        <stp>FixedRateBondzeroCouponBondCashflow</stp>
+        <stp>CT</stp>
+        <tr r="H45" s="1"/>
+        <tr r="H48" s="1"/>
+        <tr r="I51" s="1"/>
+        <tr r="I54" s="1"/>
+        <tr r="I63" s="1"/>
+        <tr r="I52" s="1"/>
+        <tr r="I42" s="1"/>
+        <tr r="H58" s="1"/>
+        <tr r="H51" s="1"/>
+        <tr r="H55" s="1"/>
+        <tr r="I46" s="1"/>
+        <tr r="H46" s="1"/>
+        <tr r="I56" s="1"/>
+        <tr r="H56" s="1"/>
+        <tr r="I59" s="1"/>
+        <tr r="H49" s="1"/>
+        <tr r="I55" s="1"/>
+        <tr r="I45" s="1"/>
+        <tr r="H42" s="1"/>
+        <tr r="H50" s="1"/>
+        <tr r="I60" s="1"/>
+        <tr r="H61" s="1"/>
+        <tr r="I44" s="1"/>
+        <tr r="H43" s="1"/>
+        <tr r="I62" s="1"/>
+        <tr r="H53" s="1"/>
+        <tr r="H63" s="1"/>
+        <tr r="H54" s="1"/>
+        <tr r="H44" s="1"/>
+        <tr r="H52" s="1"/>
+        <tr r="H47" s="1"/>
+        <tr r="I58" s="1"/>
+        <tr r="I50" s="1"/>
+        <tr r="I57" s="1"/>
+        <tr r="I53" s="1"/>
+        <tr r="H57" s="1"/>
+        <tr r="H59" s="1"/>
+        <tr r="H60" s="1"/>
+        <tr r="I47" s="1"/>
+        <tr r="I61" s="1"/>
+        <tr r="H62" s="1"/>
+        <tr r="I48" s="1"/>
+        <tr r="I49" s="1"/>
+        <tr r="I43" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>optionletvolitility</v>
+        <stp/>
+        <stp>optionletvolitility</stp>
+        <stp>0</stp>
+        <tr r="B49" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>ConstantOptionletVolatility</v>
         <stp/>
@@ -1716,34 +1715,16 @@
         <tr r="B50" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>USDLibor</v>
+        <v>s5yratehelpers</v>
         <stp/>
-        <stp>USDLibor</stp>
-        <stp>172051658</stp>
-        <tr r="J37" s="1"/>
+        <stp>s5yratehelpers</stp>
+        <stp>1362898600</stp>
+        <tr r="K30" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>optionletvolitility</v>
-        <stp/>
-        <stp>optionletvolitility</stp>
-        <stp>0</stp>
-        <tr r="B49" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>actual360</v>
-        <stp/>
-        <stp>actual360</stp>
-        <stp>372029375</stp>
-        <tr r="E48" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>s3yratehelpers</v>
         <stp/>
@@ -1752,16 +1733,7 @@
         <tr r="K29" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>102.3194216915206</v>
-        <stp/>
-        <stp>FloatingDirtyPrice</stp>
-        <stp/>
-        <tr r="D66" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>FloatingNextcoupon</v>
         <stp/>
@@ -1770,43 +1742,25 @@
         <tr r="D61" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>s5yratehelpers</v>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>4.4999999999999998E-2</v>
         <stp/>
-        <stp>s5yratehelpers</stp>
-        <stp>1362898600</stp>
-        <tr r="K30" s="1"/>
+        <stp>FixedNextcoupon</stp>
+        <stp/>
+        <tr r="C69" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>Actual365Fixed</v>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>1.5407608695652275</v>
         <stp/>
-        <stp>Actual365Fixed</stp>
-        <stp>0</stp>
-        <tr r="E50" s="1"/>
+        <stp>FixedZeroAccruedcoupon</stp>
+        <stp/>
+        <tr r="C67" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>0</v>
-        <stp/>
-        <stp>ZeroPreviouscoupon</stp>
-        <stp/>
-        <tr r="B68" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>FixedIssueDate</v>
-        <stp/>
-        <stp>FixedIssueDate</stp>
-        <stp>996172436</stp>
-        <tr r="B34" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>ZeroCleanPrice</v>
         <stp/>
@@ -1822,7 +1776,7 @@
         <tr r="K27" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>FixedRateBondzeroCouponBondCashflow</v>
         <stp/>
@@ -1831,7 +1785,52 @@
         <tr r="C63" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>FloatIssueDate</v>
+        <stp/>
+        <stp>FloatIssueDate</stp>
+        <stp>451725283</stp>
+        <tr r="B43" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>106.127528263039</v>
+        <stp/>
+        <stp>FixedCleanPrice</stp>
+        <stp/>
+        <tr r="C65" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>RemptionAmount</v>
+        <stp/>
+        <stp>RemptionAmount</stp>
+        <stp>1079574528</stp>
+        <tr r="B25" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>d1wratehelpers</v>
+        <stp/>
+        <stp>d1wratehelpers</stp>
+        <stp>1144794792</stp>
+        <tr r="K22" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>FixedNPV</v>
+        <stp/>
+        <stp>FixedNPV</stp>
+        <stp>-77321281</stp>
+        <tr r="C56" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>zeroCouponBondCashflow</v>
         <stp/>
@@ -1840,95 +1839,126 @@
         <tr r="B63" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>FixedRateBondzeroCouponBondCashflow</v>
+        <v>FixedIssueDate</v>
         <stp/>
-        <stp>FixedRateBondzeroCouponBondCashflow</stp>
-        <stp>CT</stp>
-        <tr r="I56" s="1"/>
-        <tr r="H63" s="1"/>
-        <tr r="I60" s="1"/>
-        <tr r="H58" s="1"/>
-        <tr r="H47" s="1"/>
-        <tr r="H49" s="1"/>
-        <tr r="I46" s="1"/>
-        <tr r="H56" s="1"/>
-        <tr r="H61" s="1"/>
-        <tr r="H46" s="1"/>
-        <tr r="I52" s="1"/>
-        <tr r="I62" s="1"/>
-        <tr r="H60" s="1"/>
-        <tr r="H44" s="1"/>
-        <tr r="I58" s="1"/>
-        <tr r="H48" s="1"/>
-        <tr r="I55" s="1"/>
-        <tr r="H57" s="1"/>
-        <tr r="H45" s="1"/>
-        <tr r="I42" s="1"/>
-        <tr r="H54" s="1"/>
-        <tr r="H50" s="1"/>
-        <tr r="I44" s="1"/>
-        <tr r="I59" s="1"/>
-        <tr r="H62" s="1"/>
-        <tr r="I47" s="1"/>
-        <tr r="H52" s="1"/>
-        <tr r="H42" s="1"/>
-        <tr r="I57" s="1"/>
-        <tr r="I61" s="1"/>
-        <tr r="I51" s="1"/>
-        <tr r="H53" s="1"/>
-        <tr r="H43" s="1"/>
-        <tr r="I63" s="1"/>
-        <tr r="I45" s="1"/>
-        <tr r="I50" s="1"/>
-        <tr r="H59" s="1"/>
-        <tr r="I53" s="1"/>
-        <tr r="H51" s="1"/>
-        <tr r="H55" s="1"/>
-        <tr r="I49" s="1"/>
-        <tr r="I54" s="1"/>
-        <tr r="I48" s="1"/>
-        <tr r="I43" s="1"/>
+        <stp>FixedIssueDate</stp>
+        <stp>996172436</stp>
+        <tr r="B34" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>FloatIssueDate</v>
+        <v>swFixedLegDayCounter</v>
         <stp/>
-        <stp>FloatIssueDate</stp>
-        <stp>451725283</stp>
-        <tr r="B43" s="1"/>
+        <stp>swFixedLegDayCounter</stp>
+        <stp>-748456025</stp>
+        <tr r="E45" s="1"/>
+        <tr r="E51" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>FixedNPV</v>
+        <v>bondEnginez</v>
         <stp/>
-        <stp>FixedNPV</stp>
-        <stp>-77321281</stp>
-        <tr r="C56" s="1"/>
+        <stp>bondEnginez</stp>
+        <stp>246307230</stp>
+        <tr r="B20" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>RemptionAmount</v>
+        <v>ZeroSettlementDate</v>
         <stp/>
-        <stp>RemptionAmount</stp>
-        <stp>1079574528</stp>
-        <tr r="B25" s="1"/>
+        <stp>ZeroSettlementDate</stp>
+        <stp>-1699218839</stp>
+        <tr r="B27" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>d1wratehelpers</v>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>39709</v>
         <stp/>
-        <stp>d1wratehelpers</stp>
-        <stp>1144794792</stp>
-        <tr r="K22" s="1"/>
+        <stp>+settlementDateAdjustedSer</stp>
+        <stp/>
+        <tr r="D4" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp t="s">
+        <v>floatingRateBondFixedRateBondzeroCouponBondCashflow</v>
+        <stp/>
+        <stp>floatingRateBondFixedRateBondzeroCouponBondCashflow</stp>
+        <stp>CT</stp>
+        <tr r="I70" s="1"/>
+        <tr r="I72" s="1"/>
+        <tr r="H72" s="1"/>
+        <tr r="H66" s="1"/>
+        <tr r="H69" s="1"/>
+        <tr r="H83" s="1"/>
+        <tr r="I65" s="1"/>
+        <tr r="H84" s="1"/>
+        <tr r="I82" s="1"/>
+        <tr r="I81" s="1"/>
+        <tr r="H85" s="1"/>
+        <tr r="H65" s="1"/>
+        <tr r="H76" s="1"/>
+        <tr r="H75" s="1"/>
+        <tr r="H68" s="1"/>
+        <tr r="I80" s="1"/>
+        <tr r="H80" s="1"/>
+        <tr r="H73" s="1"/>
+        <tr r="H71" s="1"/>
+        <tr r="H77" s="1"/>
+        <tr r="I83" s="1"/>
+        <tr r="I77" s="1"/>
+        <tr r="H67" s="1"/>
+        <tr r="I74" s="1"/>
+        <tr r="I84" s="1"/>
+        <tr r="I85" s="1"/>
+        <tr r="I75" s="1"/>
+        <tr r="I73" s="1"/>
+        <tr r="I66" s="1"/>
+        <tr r="I67" s="1"/>
+        <tr r="H74" s="1"/>
+        <tr r="H79" s="1"/>
+        <tr r="I79" s="1"/>
+        <tr r="I64" s="1"/>
+        <tr r="I78" s="1"/>
+        <tr r="H82" s="1"/>
+        <tr r="H78" s="1"/>
+        <tr r="I68" s="1"/>
+        <tr r="H81" s="1"/>
+        <tr r="I71" s="1"/>
+        <tr r="H70" s="1"/>
+        <tr r="H64" s="1"/>
+        <tr r="I69" s="1"/>
+        <tr r="I76" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>USgovi</v>
+        <stp/>
+        <stp>USgovi</stp>
+        <stp>814714544</stp>
+        <tr r="E38" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>FixedYield</v>
+        <stp/>
+        <stp>FixedYield</stp>
+        <stp>-1293104115</stp>
+        <tr r="C62" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d3mratehelpers</v>
+        <stp/>
+        <stp>d3mratehelpers</stp>
+        <stp>1144794792</stp>
+        <tr r="K24" s="1"/>
+      </tp>
       <tp t="s">
         <v>USDLibor1</v>
         <stp/>
@@ -1937,52 +1967,7 @@
         <tr r="J39" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>USgovi</v>
-        <stp/>
-        <stp>USgovi</stp>
-        <stp>814714544</stp>
-        <tr r="E38" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>bondEnginez</v>
-        <stp/>
-        <stp>bondEnginez</stp>
-        <stp>246307230</stp>
-        <tr r="B20" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>ZeroSettlementDate</v>
-        <stp/>
-        <stp>ZeroSettlementDate</stp>
-        <stp>-1699218839</stp>
-        <tr r="B27" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>d3mratehelpers</v>
-        <stp/>
-        <stp>d3mratehelpers</stp>
-        <stp>1144794792</stp>
-        <tr r="K24" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>101.75730882512499</v>
-        <stp/>
-        <stp>FloatingCleanPrice</stp>
-        <stp/>
-        <tr r="D65" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>zc6mPeriod</v>
         <stp/>
@@ -1990,6 +1975,8 @@
         <stp>-1226026161</stp>
         <tr r="E9" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>zc3mPeriod</v>
         <stp/>
@@ -1998,25 +1985,48 @@
         <tr r="E8" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>FixedYield</v>
+        <v>zc6m</v>
         <stp/>
-        <stp>FixedYield</stp>
-        <stp>-1293104115</stp>
-        <tr r="C62" s="1"/>
+        <stp>zc6m</stp>
+        <stp>-792237096</stp>
+        <tr r="H9" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d9mratehelpers</v>
+        <stp/>
+        <stp>d9mratehelpers</stp>
+        <stp>-969134424</stp>
+        <tr r="K26" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>forwardStart</v>
+        <stp/>
+        <stp>forwardStart</stp>
+        <stp>-223693829</stp>
+        <tr r="E47" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
-      <tp>
-        <v>3.4298412186850417E-2</v>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>zcBondsDayCounter</v>
         <stp/>
-        <stp>FloatingNextcoupon</stp>
-        <stp/>
-        <tr r="D69" s="1"/>
+        <stp>zcBondsDayCounter</stp>
+        <stp>0</stp>
+        <tr r="B9" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>86.317292342665496</v>
+        <stp/>
+        <stp>ZeroNPV</stp>
+        <stp/>
+        <tr r="B64" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>d6mratehelpers</v>
         <stp/>
@@ -2025,92 +2035,67 @@
         <tr r="K25" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>d9mratehelpers</v>
+        <v>s10y</v>
         <stp/>
-        <stp>d9mratehelpers</stp>
-        <stp>-969134424</stp>
-        <tr r="K26" s="1"/>
+        <stp>s10y</stp>
+        <stp>1121190872</stp>
+        <tr r="H31" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.afca8c951de84249a6b2e7527de93d34">
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
-        <v>floatingRateBondFixedRateBondzeroCouponBondCashflow</v>
+        <v>depositDayCounter</v>
         <stp/>
-        <stp>floatingRateBondFixedRateBondzeroCouponBondCashflow</stp>
-        <stp>CT</stp>
-        <tr r="H78" s="1"/>
-        <tr r="H70" s="1"/>
-        <tr r="I72" s="1"/>
-        <tr r="I74" s="1"/>
-        <tr r="I78" s="1"/>
-        <tr r="I67" s="1"/>
-        <tr r="H82" s="1"/>
-        <tr r="H84" s="1"/>
-        <tr r="I83" s="1"/>
-        <tr r="H74" s="1"/>
-        <tr r="H72" s="1"/>
-        <tr r="I64" s="1"/>
-        <tr r="H69" s="1"/>
-        <tr r="H85" s="1"/>
-        <tr r="I69" s="1"/>
-        <tr r="H83" s="1"/>
-        <tr r="H77" s="1"/>
-        <tr r="I85" s="1"/>
-        <tr r="H67" s="1"/>
-        <tr r="H68" s="1"/>
-        <tr r="I70" s="1"/>
-        <tr r="I77" s="1"/>
-        <tr r="I75" s="1"/>
-        <tr r="H64" s="1"/>
-        <tr r="H71" s="1"/>
-        <tr r="H75" s="1"/>
-        <tr r="I82" s="1"/>
-        <tr r="I84" s="1"/>
-        <tr r="H66" s="1"/>
-        <tr r="I65" s="1"/>
-        <tr r="H80" s="1"/>
-        <tr r="H73" s="1"/>
-        <tr r="I66" s="1"/>
-        <tr r="I81" s="1"/>
-        <tr r="I76" s="1"/>
-        <tr r="H81" s="1"/>
-        <tr r="I73" s="1"/>
-        <tr r="H76" s="1"/>
-        <tr r="I79" s="1"/>
-        <tr r="I80" s="1"/>
-        <tr r="H79" s="1"/>
-        <tr r="H65" s="1"/>
-        <tr r="I71" s="1"/>
-        <tr r="I68" s="1"/>
+        <stp>depositDayCounter</stp>
+        <stp>372029375</stp>
+        <tr r="E43" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>107.66828913260423</v>
+        <stp/>
+        <stp>FixedDirtyPrice</stp>
+        <stp/>
+        <tr r="C66" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>loglinier</v>
+        <stp/>
+        <stp>loglinier</stp>
+        <stp>0</stp>
+        <tr r="E44" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+      <tp>
+        <v>107.66828913260423</v>
+        <stp/>
+        <stp>FixedNPV</stp>
+        <stp/>
+        <tr r="C64" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+      <tp t="s">
+        <v>ZeroDirtyPrice</v>
+        <stp/>
+        <stp>ZeroDirtyPrice</stp>
+        <stp>1001970241</stp>
+        <tr r="B58" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>floatingRateBondFixedRateBondzeroCouponBondCashflow</v>
         <stp/>
         <stp>floatingRateBondFixedRateBondzeroCouponBondCashflow</stp>
         <stp>588410313</stp>
         <tr r="D63" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>FloatingFixedZeroPreviouscoupon</v>
-        <stp/>
-        <stp>FloatingFixedZeroPreviouscoupon</stp>
-        <stp>-1208119139</stp>
-        <tr r="D60" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a299567c0f8b4fec933b2b6f314f9629">
-      <tp t="s">
-        <v>ZeroDirtyPrice</v>
-        <stp/>
-        <stp>ZeroDirtyPrice</stp>
-        <stp>1001970241</stp>
-        <tr r="B58" s="1"/>
       </tp>
     </main>
   </volType>
@@ -2452,8 +2437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28025E14-2DBA-4FA2-A060-A0CB22BD8F4F}">
   <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3900,7 +3885,7 @@
       </c>
       <c r="B61" t="str">
         <f>+_xll._Bond_nextCouponRate(B$55&amp;$A61,B54)</f>
-        <v>#no coupon paid at cashflow date 15/08/2013</v>
+        <v>ZeroNextcoupon</v>
       </c>
       <c r="C61" t="str">
         <f>+_xll._Bond_nextCouponRate(C$55&amp;$A61,C54)</f>
@@ -4094,7 +4079,7 @@
       </c>
       <c r="B69" t="str">
         <f>+_xll._Value(B61)</f>
-        <v>#NA</v>
+        <v>#no coupon paid at cashflow date 15/08/2013 ,Bond.nextCouponRate</v>
       </c>
       <c r="C69">
         <f>+_xll._Value(C61)</f>

</xml_diff>

<commit_message>
resolve boundary cyclic dependancy check
</commit_message>
<xml_diff>
--- a/Cephei.XL/Bond1.xlsx
+++ b/Cephei.XL/Bond1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\source\repos\Cephei2\Cephei.XL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0284BD8-A35D-4364-8F53-4583EE87BAF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66AB403-043B-4B07-9235-ABD4574C7D08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1287AFFA-50F8-48B2-8168-E284DC333339}"/>
   </bookViews>
@@ -558,23 +558,123 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>zc1y</v>
+        <v>FloatingFixedZeroAccruedcoupon</v>
         <stp/>
-        <stp>zc1y</stp>
-        <stp>-2050528296</stp>
-        <tr r="H10" s="1"/>
+        <stp>FloatingFixedZeroAccruedcoupon</stp>
+        <stp>-1208119139</stp>
+        <tr r="D59" s="1"/>
       </tp>
       <tp t="s">
-        <v>Semiannual</v>
+        <v>floatingRateBond</v>
         <stp/>
-        <stp>Semiannual</stp>
-        <stp>1704154923</stp>
-        <tr r="E39" s="1"/>
+        <stp>floatingRateBond</stp>
+        <stp>-922790952</stp>
+        <tr r="B47" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>d1mratehelpers</v>
+        <stp/>
+        <stp>d1mratehelpers</stp>
+        <stp>-1371787608</stp>
+        <tr r="K23" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>3.0058566999435425E-2</v>
+        <stp/>
+        <stp>ZeroYield</stp>
+        <stp/>
+        <tr r="B70" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>ZeroAccruedcoupon</v>
+        <stp/>
+        <stp>ZeroAccruedcoupon</stp>
+        <stp>1029105693</stp>
+        <tr r="B59" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>Quarterly</v>
+        <stp/>
+        <stp>Quarterly</stp>
+        <stp>-302169631</stp>
+        <tr r="E49" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>s10yratehelpers</v>
+        <stp/>
+        <stp>s10yratehelpers</stp>
+        <stp>154939048</stp>
+        <tr r="K31" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>schedule1</v>
+        <stp/>
+        <stp>schedule1</stp>
+        <stp>1913417000</stp>
+        <tr r="L15" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>schedule0</v>
+        <stp/>
+        <stp>schedule0</stp>
+        <stp>1913417000</stp>
+        <tr r="L14" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>schedule3</v>
+        <stp/>
+        <stp>schedule3</stp>
+        <stp>1913417000</stp>
+        <tr r="L17" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>schedule2</v>
+        <stp/>
+        <stp>schedule2</stp>
+        <stp>1913417000</stp>
+        <tr r="L16" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>schedule4</v>
+        <stp/>
+        <stp>schedule4</stp>
+        <stp>1913417000</stp>
+        <tr r="L18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FloatingNPV</v>
+        <stp/>
+        <stp>FloatingNPV</stp>
+        <stp>588410313</stp>
+        <tr r="D56" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>todaysDateSer</v>
+        <stp/>
+        <stp>todaysDateSer</stp>
+        <stp>-1204259704</stp>
+        <tr r="C8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
         <v>+settlementDate</v>
         <stp/>
@@ -583,139 +683,617 @@
         <tr r="B3" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>d1mratehelpers</v>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>0</v>
         <stp/>
-        <stp>d1mratehelpers</stp>
-        <stp>-1371787608</stp>
-        <tr r="K23" s="1"/>
+        <stp>ZeroAccruedcoupon</stp>
+        <stp/>
+        <tr r="B67" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>floatingRateBond</v>
+        <v>s15yratehelpers</v>
         <stp/>
-        <stp>floatingRateBond</stp>
-        <stp>-922790952</stp>
-        <tr r="B47" s="1"/>
+        <stp>s15yratehelpers</stp>
+        <stp>-96719192</stp>
+        <tr r="K32" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>bondDiscountingTermStructure</v>
+        <v>settlementDays</v>
         <stp/>
-        <stp>bondDiscountingTermStructure</stp>
-        <stp>-1358081960</stp>
-        <tr r="B17" s="1"/>
+        <stp>settlementDays</stp>
+        <stp>3</stp>
+        <tr r="B6" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>zc3m</v>
+        <v>zc1yPeriod</v>
         <stp/>
-        <stp>zc3m</stp>
-        <stp>-1010340904</stp>
-        <tr r="H8" s="1"/>
+        <stp>zc1yPeriod</stp>
+        <stp>2119925464</stp>
+        <tr r="E10" s="1"/>
       </tp>
       <tp t="s">
-        <v>FixedZeroPreviouscoupon</v>
+        <v>zeroCouponBond</v>
         <stp/>
-        <stp>FixedZeroPreviouscoupon</stp>
-        <stp>815396861</stp>
-        <tr r="C60" s="1"/>
+        <stp>zeroCouponBond</stp>
+        <stp>-762789832</stp>
+        <tr r="B29" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>floatcouponpricer2</v>
+        <v>ActualActualBond</v>
         <stp/>
-        <stp>floatcouponpricer2</stp>
-        <stp>1878722209</stp>
-        <tr r="B51" s="1"/>
+        <stp>ActualActualBond</stp>
+        <stp>1506851973</stp>
+        <tr r="E40" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>FloatSettlementDatte</v>
+        <stp/>
+        <stp>FloatSettlementDatte</stp>
+        <stp>888501985</stp>
+        <tr r="B42" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>+settlementDateAdjustedSer</v>
+        <v>ZeroIssueDate</v>
         <stp/>
-        <stp>+settlementDateAdjustedSer</stp>
-        <stp>-649169906</stp>
-        <tr r="C4" s="1"/>
+        <stp>ZeroIssueDate</stp>
+        <stp>-12167724</stp>
+        <tr r="B28" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>102.3194216915206</v>
+        <stp/>
+        <stp>FloatingNPV</stp>
+        <stp/>
+        <tr r="D64" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>libor3mPeriod</v>
+        <stp/>
+        <stp>libor3mPeriod</stp>
+        <stp>-1226026113</stp>
+        <tr r="B40" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>depoSwapTermStructure</v>
+        <stp/>
+        <stp>depoSwapTermStructure</stp>
+        <stp>-1492299688</stp>
+        <tr r="B19" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>3.6475570816152846E-2</v>
+        <stp/>
+        <stp>FixedYield</stp>
+        <stp/>
+        <tr r="C70" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>floatcouponpricer</v>
+        <stp/>
+        <stp>floatcouponpricer</stp>
+        <stp>1741592878</stp>
+        <tr r="B48" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FixedZeroAccruedcoupon</v>
+        <stp/>
+        <stp>FixedZeroAccruedcoupon</stp>
+        <stp>815396861</stp>
+        <tr r="C59" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>Gearing</v>
+        <stp/>
+        <stp>Gearing</stp>
+        <stp>1072693248</stp>
+        <tr r="B44" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>107.66828913260423</v>
+        <stp/>
+        <stp>FixedNPV</stp>
+        <stp/>
+        <tr r="C64" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>bondEnginez</v>
+        <stp/>
+        <stp>bondEnginez</stp>
+        <stp>246307230</stp>
+        <tr r="B20" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>3.4298412186850417E-2</v>
+        <stp/>
+        <stp>FloatingNextcoupon</stp>
+        <stp/>
+        <tr r="D69" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FixedRedemption</v>
+        <stp/>
+        <stp>FixedRedemption</stp>
+        <stp>1079574528</stp>
+        <tr r="B32" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FloatRedemption</v>
+        <stp/>
+        <stp>FloatRedemption</stp>
+        <stp>1079574528</stp>
+        <tr r="B41" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>d3mratehelpers</v>
+        <stp/>
+        <stp>d3mratehelpers</stp>
+        <stp>1144794792</stp>
+        <tr r="K24" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp t="s">
+        <v>floatingRateBondFixedRateBondzeroCouponBondCashflow</v>
+        <stp/>
+        <stp>floatingRateBondFixedRateBondzeroCouponBondCashflow</stp>
+        <stp>CT</stp>
+        <tr r="I84" s="1"/>
+        <tr r="H70" s="1"/>
+        <tr r="H74" s="1"/>
+        <tr r="H66" s="1"/>
+        <tr r="I80" s="1"/>
+        <tr r="I76" s="1"/>
+        <tr r="H64" s="1"/>
+        <tr r="I77" s="1"/>
+        <tr r="I81" s="1"/>
+        <tr r="I65" s="1"/>
+        <tr r="I72" s="1"/>
+        <tr r="H81" s="1"/>
+        <tr r="H80" s="1"/>
+        <tr r="I82" s="1"/>
+        <tr r="I66" s="1"/>
+        <tr r="I68" s="1"/>
+        <tr r="H69" s="1"/>
+        <tr r="I71" s="1"/>
+        <tr r="H85" s="1"/>
+        <tr r="H82" s="1"/>
+        <tr r="I67" s="1"/>
+        <tr r="H84" s="1"/>
+        <tr r="H76" s="1"/>
+        <tr r="H65" s="1"/>
+        <tr r="I74" s="1"/>
+        <tr r="H67" s="1"/>
+        <tr r="H79" s="1"/>
+        <tr r="H78" s="1"/>
+        <tr r="I75" s="1"/>
+        <tr r="H71" s="1"/>
+        <tr r="I64" s="1"/>
+        <tr r="H77" s="1"/>
+        <tr r="I70" s="1"/>
+        <tr r="H72" s="1"/>
+        <tr r="I79" s="1"/>
+        <tr r="H83" s="1"/>
+        <tr r="I85" s="1"/>
+        <tr r="H73" s="1"/>
+        <tr r="H68" s="1"/>
+        <tr r="I78" s="1"/>
+        <tr r="H75" s="1"/>
+        <tr r="I83" s="1"/>
+        <tr r="I69" s="1"/>
+        <tr r="I73" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>+settlementDateAdjusted</v>
+        <stp/>
+        <stp>+settlementDateAdjusted</stp>
+        <stp>-544419191</stp>
+        <tr r="B4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>d9mratehelpers</v>
+        <stp/>
+        <stp>d9mratehelpers</stp>
+        <stp>-969134424</stp>
+        <tr r="K26" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>s15y</v>
+        <stp/>
+        <stp>s15y</stp>
+        <stp>772304968</stp>
+        <tr r="H32" s="1"/>
       </tp>
       <tp t="s">
-        <v>faceAmount</v>
+        <v>d6mratehelpers</v>
         <stp/>
-        <stp>faceAmount</stp>
-        <stp>1079574528</stp>
-        <tr r="B24" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>swFloatingLegIndex</v>
-        <stp/>
-        <stp>swFloatingLegIndex</stp>
-        <stp>0</stp>
-        <tr r="E46" s="1"/>
+        <stp>d6mratehelpers</stp>
+        <stp>-449040728</stp>
+        <tr r="K25" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>d9mRate</v>
-        <stp/>
-        <stp>d9mRate</stp>
-        <stp>0</stp>
-        <tr r="J26" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d1mRate</v>
-        <stp/>
-        <stp>d1mRate</stp>
-        <stp>0</stp>
-        <tr r="J23" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d3mRate</v>
-        <stp/>
-        <stp>d3mRate</stp>
-        <stp>0</stp>
-        <tr r="J24" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d6mRate</v>
-        <stp/>
-        <stp>d6mRate</stp>
-        <stp>0</stp>
-        <tr r="J25" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>ZeroNextcoupon</v>
+        <v>#no coupon paid at cashflow date 15/08/2013</v>
         <stp/>
         <stp>ZeroNextcoupon</stp>
-        <stp>1029105693#</stp>
+        <stp>1029105693</stp>
         <tr r="B61" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>FloatingFixedZeroAccruedcoupon</v>
+        <v>USDLibor1</v>
         <stp/>
-        <stp>FloatingFixedZeroAccruedcoupon</stp>
-        <stp>-1208119139</stp>
-        <tr r="D59" s="1"/>
+        <stp>USDLibor1</stp>
+        <stp>2003614270</stp>
+        <tr r="J39" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>floatingBondSchedule</v>
+        <v>ZeroDirtyPrice</v>
         <stp/>
-        <stp>floatingBondSchedule</stp>
-        <stp>-2089128530</stp>
-        <tr r="B46" s="1"/>
+        <stp>ZeroDirtyPrice</stp>
+        <stp>1001970241</stp>
+        <tr r="B58" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>USgovi</v>
+        <stp/>
+        <stp>USgovi</stp>
+        <stp>814714544</stp>
+        <tr r="E38" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>101.75730882512499</v>
+        <stp/>
+        <stp>FloatingCleanPrice</stp>
+        <stp/>
+        <tr r="D65" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FloatingFixedZeroPreviouscoupon</v>
+        <stp/>
+        <stp>FloatingFixedZeroPreviouscoupon</stp>
+        <stp>-1208119139</stp>
+        <tr r="D60" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>bondInstruments</v>
+        <stp/>
+        <stp>bondInstruments</stp>
+        <stp>1882299273</stp>
+        <tr r="B16" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>floatingRateBondFixedRateBondzeroCouponBondCashflow</v>
+        <stp/>
+        <stp>floatingRateBondFixedRateBondzeroCouponBondCashflow</stp>
+        <stp>588410313</stp>
+        <tr r="D63" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FloatIssueDate</v>
+        <stp/>
+        <stp>FloatIssueDate</stp>
+        <stp>451725283</stp>
+        <tr r="B43" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp t="s">
+        <v>FixedRateBondzeroCouponBondCashflow</v>
+        <stp/>
+        <stp>FixedRateBondzeroCouponBondCashflow</stp>
+        <stp>CT</stp>
+        <tr r="H42" s="1"/>
+        <tr r="H60" s="1"/>
+        <tr r="I47" s="1"/>
+        <tr r="H61" s="1"/>
+        <tr r="H52" s="1"/>
+        <tr r="H48" s="1"/>
+        <tr r="H43" s="1"/>
+        <tr r="I52" s="1"/>
+        <tr r="H45" s="1"/>
+        <tr r="I57" s="1"/>
+        <tr r="I55" s="1"/>
+        <tr r="H59" s="1"/>
+        <tr r="I60" s="1"/>
+        <tr r="I49" s="1"/>
+        <tr r="I45" s="1"/>
+        <tr r="I58" s="1"/>
+        <tr r="I63" s="1"/>
+        <tr r="H46" s="1"/>
+        <tr r="H63" s="1"/>
+        <tr r="H51" s="1"/>
+        <tr r="I59" s="1"/>
+        <tr r="H62" s="1"/>
+        <tr r="I43" s="1"/>
+        <tr r="I42" s="1"/>
+        <tr r="I51" s="1"/>
+        <tr r="H56" s="1"/>
+        <tr r="H55" s="1"/>
+        <tr r="I56" s="1"/>
+        <tr r="H44" s="1"/>
+        <tr r="H54" s="1"/>
+        <tr r="I54" s="1"/>
+        <tr r="H49" s="1"/>
+        <tr r="I48" s="1"/>
+        <tr r="I50" s="1"/>
+        <tr r="H57" s="1"/>
+        <tr r="H50" s="1"/>
+        <tr r="H53" s="1"/>
+        <tr r="H58" s="1"/>
+        <tr r="I46" s="1"/>
+        <tr r="I61" s="1"/>
+        <tr r="H47" s="1"/>
+        <tr r="I53" s="1"/>
+        <tr r="I62" s="1"/>
+        <tr r="I44" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>actual360</v>
+        <stp/>
+        <stp>actual360</stp>
+        <stp>372029375</stp>
+        <tr r="E48" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>optionletvolitility</v>
+        <stp/>
+        <stp>optionletvolitility</stp>
+        <stp>0</stp>
+        <tr r="B49" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FixedRateCoupon</v>
+        <stp/>
+        <stp>FixedRateCoupon</stp>
+        <stp>1325718839</stp>
+        <tr r="B36" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>bondEnginefi</v>
+        <stp/>
+        <stp>bondEnginefi</stp>
+        <stp>246307230</stp>
+        <tr r="B21" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>ConstantOptionletVolatility</v>
+        <stp/>
+        <stp>ConstantOptionletVolatility</stp>
+        <stp>315382730</stp>
+        <tr r="B50" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FixedIssueDate</v>
+        <stp/>
+        <stp>FixedIssueDate</stp>
+        <stp>996172436</stp>
+        <tr r="B34" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>s5yratehelpers</v>
+        <stp/>
+        <stp>s5yratehelpers</stp>
+        <stp>1362898600</stp>
+        <tr r="K30" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>bondEnginefl</v>
+        <stp/>
+        <stp>bondEnginefl</stp>
+        <stp>246307230</stp>
+        <tr r="B22" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>s3yratehelpers</v>
+        <stp/>
+        <stp>s3yratehelpers</stp>
+        <stp>-751030616</stp>
+        <tr r="K29" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>Spreads</v>
+        <stp/>
+        <stp>Spreads</stp>
+        <stp>-308163663</stp>
+        <tr r="B45" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>d1yratehelpers</v>
+        <stp/>
+        <stp>d1yratehelpers</stp>
+        <stp>-499372376</stp>
+        <tr r="K27" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>ZeroCleanPrice</v>
+        <stp/>
+        <stp>ZeroCleanPrice</stp>
+        <stp>1001970241</stp>
+        <tr r="B57" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FixedRateBondzeroCouponBondCashflow</v>
+        <stp/>
+        <stp>FixedRateBondzeroCouponBondCashflow</stp>
+        <stp>-77321281</stp>
+        <tr r="C63" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>Actual365Fixed</v>
+        <stp/>
+        <stp>Actual365Fixed</stp>
+        <stp>0</stp>
+        <tr r="E50" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>RemptionAmount</v>
+        <stp/>
+        <stp>RemptionAmount</stp>
+        <stp>1079574528</stp>
+        <tr r="B25" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d1wratehelpers</v>
+        <stp/>
+        <stp>d1wratehelpers</stp>
+        <stp>1144794792</stp>
+        <tr r="K22" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>termStructureDayCounter</v>
+        <stp/>
+        <stp>termStructureDayCounter</stp>
+        <stp>1443485125</stp>
+        <tr r="E41" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>ZeroPreviouscoupon</stp>
+        <stp/>
+        <tr r="B68" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>102.3194216915206</v>
+        <stp/>
+        <stp>FloatingDirtyPrice</stp>
+        <stp/>
+        <tr r="D66" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>ZeroNPV</v>
+        <stp/>
+        <stp>ZeroNPV</stp>
+        <stp>1001970241</stp>
+        <tr r="B56" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>zeroCouponBondCashflow</v>
+        <stp/>
+        <stp>zeroCouponBondCashflow</stp>
+        <stp>1001970241</stp>
+        <tr r="B63" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>Fixing1</v>
+        <stp/>
+        <stp>Fixing1</stp>
+        <stp>1755687198</stp>
+        <tr r="J39" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>discount</v>
+        <stp/>
+        <stp>discount</stp>
+        <stp>0</stp>
+        <tr r="E42" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>calendar</v>
+        <stp/>
+        <stp>calendar</stp>
+        <stp>0</stp>
+        <tr r="B2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
         <v>redemption</v>
         <stp/>
@@ -723,15 +1301,26 @@
         <stp>1079574528</stp>
         <tr r="B13" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>s2yratehelpers</v>
+        <v>FloatingCleanPrice</v>
         <stp/>
-        <stp>s2yratehelpers</stp>
-        <stp>-63164760</stp>
-        <tr r="K28" s="1"/>
+        <stp>FloatingCleanPrice</stp>
+        <stp>588410313</stp>
+        <tr r="D57" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>couponRate4</v>
+        <stp/>
+        <stp>couponRate4</stp>
+        <stp>1325718839</stp>
+        <tr r="J18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
         <v>d1wRate</v>
         <stp/>
@@ -740,16 +1329,16 @@
         <tr r="J22" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>3.6475570816152846E-2</v>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FloatingDirtyPrice</v>
         <stp/>
-        <stp>FixedYield</stp>
-        <stp/>
-        <tr r="C70" s="1"/>
+        <stp>FloatingDirtyPrice</stp>
+        <stp>588410313</stp>
+        <tr r="D58" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
         <v>ZeroPreviouscoupon</v>
         <stp/>
@@ -758,7 +1347,25 @@
         <tr r="B60" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>bondhelper4</v>
+        <stp/>
+        <stp>bondhelper4</stp>
+        <stp>-1090572417</stp>
+        <tr r="M18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>86.317292342665496</v>
+        <stp/>
+        <stp>ZeroCleanPrice</stp>
+        <stp/>
+        <tr r="B65" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
         <v>FixedNextcoupon</v>
         <stp/>
@@ -767,38 +1374,29 @@
         <tr r="C61" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>ActualActualBond</v>
+        <v>couponRate3</v>
         <stp/>
-        <stp>ActualActualBond</stp>
-        <stp>1506851973</stp>
-        <tr r="E40" s="1"/>
+        <stp>couponRate3</stp>
+        <stp>2013949594</stp>
+        <tr r="J17" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>102.3194216915206</v>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>s2yRate</v>
         <stp/>
-        <stp>FloatingNPV</stp>
-        <stp/>
-        <tr r="D64" s="1"/>
+        <stp>s2yRate</stp>
+        <stp>0</stp>
+        <tr r="J28" s="1"/>
       </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>s3yRate</v>
         <stp/>
         <stp>s3yRate</stp>
         <stp>0</stp>
         <tr r="J29" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>s2yRate</v>
-        <stp/>
-        <stp>s2yRate</stp>
-        <stp>0</stp>
-        <tr r="J28" s="1"/>
       </tp>
       <tp t="s">
         <v>s5yRate</v>
@@ -814,415 +1412,8 @@
         <stp>0</stp>
         <tr r="J27" s="1"/>
       </tp>
-      <tp t="s">
-        <v>FloatingCleanPrice</v>
-        <stp/>
-        <stp>FloatingCleanPrice</stp>
-        <stp>588410313</stp>
-        <tr r="D57" s="1"/>
-      </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>ZeroIssueDate</v>
-        <stp/>
-        <stp>ZeroIssueDate</stp>
-        <stp>-12167724</stp>
-        <tr r="B28" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FloatingDirtyPrice</v>
-        <stp/>
-        <stp>FloatingDirtyPrice</stp>
-        <stp>588410313</stp>
-        <tr r="D58" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FloatSettlementDatte</v>
-        <stp/>
-        <stp>FloatSettlementDatte</stp>
-        <stp>888501985</stp>
-        <tr r="B42" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FixedCleanPrice</v>
-        <stp/>
-        <stp>FixedCleanPrice</stp>
-        <stp>-77321281</stp>
-        <tr r="C57" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>bondInstruments</v>
-        <stp/>
-        <stp>bondInstruments</stp>
-        <stp>1882299273</stp>
-        <tr r="B16" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>tolerance</v>
-        <stp/>
-        <stp>tolerance</stp>
-        <stp>-1573562951</stp>
-        <tr r="B14" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>+settlementDateAdjusted</v>
-        <stp/>
-        <stp>+settlementDateAdjusted</stp>
-        <stp>-544419191</stp>
-        <tr r="B4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>todaysDate</v>
-        <stp/>
-        <stp>todaysDate</stp>
-        <stp>-111422835</stp>
-        <tr r="B8" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>s15y</v>
-        <stp/>
-        <stp>s15y</stp>
-        <stp>772304968</stp>
-        <tr r="H32" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>FloatingFixedZeroPreviouscoupon</v>
-        <stp/>
-        <stp>FloatingFixedZeroPreviouscoupon</stp>
-        <stp>-1208119139</stp>
-        <tr r="D60" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>101.75730882512499</v>
-        <stp/>
-        <stp>FloatingCleanPrice</stp>
-        <stp/>
-        <tr r="D65" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>fixedBondSchedule</v>
-        <stp/>
-        <stp>fixedBondSchedule</stp>
-        <stp>-2089128530</stp>
-        <tr r="B35" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FixedDirtyPrice</v>
-        <stp/>
-        <stp>FixedDirtyPrice</stp>
-        <stp>-77321281</stp>
-        <tr r="C58" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FloatingYield</v>
-        <stp/>
-        <stp>FloatingYield</stp>
-        <stp>-712193011</stp>
-        <tr r="D62" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>3.4298412186850417E-2</v>
-        <stp/>
-        <stp>FloatingNextcoupon</stp>
-        <stp/>
-        <tr r="D69" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FloatRedemption</v>
-        <stp/>
-        <stp>FloatRedemption</stp>
-        <stp>1079574528</stp>
-        <tr r="B41" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>Gearing</v>
-        <stp/>
-        <stp>Gearing</stp>
-        <stp>1072693248</stp>
-        <tr r="B44" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FixedRedemption</v>
-        <stp/>
-        <stp>FixedRedemption</stp>
-        <stp>1079574528</stp>
-        <tr r="B32" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>fixingDays</v>
-        <stp/>
-        <stp>fixingDays</stp>
-        <stp>3</stp>
-        <tr r="B5" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>bondhelper3</v>
-        <stp/>
-        <stp>bondhelper3</stp>
-        <stp>922693503</stp>
-        <tr r="M17" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>termStructureDayCounter</v>
-        <stp/>
-        <stp>termStructureDayCounter</stp>
-        <stp>1443485125</stp>
-        <tr r="E41" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>ZeroNPV</v>
-        <stp/>
-        <stp>ZeroNPV</stp>
-        <stp>1001970241</stp>
-        <tr r="B56" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>fixingDaysNeg</v>
-        <stp/>
-        <stp>fixingDaysNeg</stp>
-        <stp>-3</stp>
-        <tr r="B7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>Fixing1</v>
-        <stp/>
-        <stp>Fixing1</stp>
-        <stp>1755687198</stp>
-        <tr r="J39" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>Spreads</v>
-        <stp/>
-        <stp>Spreads</stp>
-        <stp>-308163663</stp>
-        <tr r="B45" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>0</v>
-        <stp/>
-        <stp>ZeroPreviouscoupon</stp>
-        <stp/>
-        <tr r="B68" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>102.3194216915206</v>
-        <stp/>
-        <stp>FloatingDirtyPrice</stp>
-        <stp/>
-        <tr r="D66" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FixedRateBond</v>
-        <stp/>
-        <stp>FixedRateBond</stp>
-        <stp>1820916808</stp>
-        <tr r="B37" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>39706</v>
-        <stp/>
-        <stp>todaysDateSer</stp>
-        <stp/>
-        <tr r="D8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>2.2009365270878184E-2</v>
-        <stp/>
-        <stp>FloatingYield</stp>
-        <stp/>
-        <tr r="D70" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>bondEnginefl</v>
-        <stp/>
-        <stp>bondEnginefl</stp>
-        <stp>246307230</stp>
-        <tr r="B22" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>actual360</v>
-        <stp/>
-        <stp>actual360</stp>
-        <stp>372029375</stp>
-        <tr r="E48" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FixedRateCoupon</v>
-        <stp/>
-        <stp>FixedRateCoupon</stp>
-        <stp>1325718839</stp>
-        <tr r="B36" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>bondEnginefi</v>
-        <stp/>
-        <stp>bondEnginefi</stp>
-        <stp>246307230</stp>
-        <tr r="B21" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ZeroYield</v>
-        <stp/>
-        <stp>ZeroYield</stp>
-        <stp>-1391670259</stp>
-        <tr r="B62" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>bondhelper0</v>
-        <stp/>
-        <stp>bondhelper0</stp>
-        <stp>1862217599</stp>
-        <tr r="M14" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>depoSwapInstruments</v>
-        <stp/>
-        <stp>depoSwapInstruments</stp>
-        <stp>-501517731</stp>
-        <tr r="B18" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp t="s">
-        <v>#no coupon paid at cashflow date 15/08/2013 ,Bond.nextCouponRate</v>
-        <stp/>
-        <stp>ZeroNextcoupon</stp>
-        <stp/>
-        <tr r="B69" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>zc1yPeriod</v>
-        <stp/>
-        <stp>zc1yPeriod</stp>
-        <stp>2119925464</stp>
-        <tr r="E10" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>zeroCouponBond</v>
-        <stp/>
-        <stp>zeroCouponBond</stp>
-        <stp>-762789832</stp>
-        <tr r="B29" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>couponRate1</v>
-        <stp/>
-        <stp>couponRate1</stp>
-        <stp>1162275258</stp>
-        <tr r="J15" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>couponRate3</v>
-        <stp/>
-        <stp>couponRate3</stp>
-        <stp>2013949594</stp>
-        <tr r="J17" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d1m</v>
-        <stp/>
-        <stp>d1m</stp>
-        <stp>-1226026145</stp>
-        <tr r="H23" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>d6m</v>
-        <stp/>
-        <stp>d6m</stp>
-        <stp>-1226026161</stp>
-        <tr r="H25" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>d3m</v>
-        <stp/>
-        <stp>d3m</stp>
-        <stp>-1226026113</stp>
-        <tr r="H24" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>d9m</v>
-        <stp/>
-        <stp>d9m</stp>
-        <stp>-1226026273</stp>
-        <tr r="H26" s="1"/>
-      </tp>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
         <v>bondhelper1</v>
         <stp/>
@@ -1231,7 +1422,7 @@
         <tr r="M15" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
         <v>instruments</v>
         <stp/>
@@ -1239,30 +1430,23 @@
         <stp>-192993751</stp>
         <tr r="B15" s="1"/>
       </tp>
-      <tp t="s">
-        <v>FixedZeroAccruedcoupon</v>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>4.4999999999999998E-2</v>
         <stp/>
-        <stp>FixedZeroAccruedcoupon</stp>
-        <stp>815396861</stp>
-        <tr r="C59" s="1"/>
+        <stp>FixedZeroPreviouscoupon</stp>
+        <stp/>
+        <tr r="C68" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>bondhelper2</v>
+        <v>floatingBondSchedule</v>
         <stp/>
-        <stp>bondhelper2</stp>
-        <stp>-1677774977</stp>
-        <tr r="M16" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>zc1yRate</v>
-        <stp/>
-        <stp>zc1yRate</stp>
-        <stp>0</stp>
-        <tr r="B12" s="1"/>
+        <stp>floatingBondSchedule</stp>
+        <stp>-2089128530</stp>
+        <tr r="B46" s="1"/>
       </tp>
       <tp t="s">
         <v>s10yRate</v>
@@ -1279,14 +1463,23 @@
         <tr r="J32" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>floatcouponpricer</v>
+        <v>zc1yRate</v>
         <stp/>
-        <stp>floatcouponpricer</stp>
-        <stp>1741592878</stp>
-        <tr r="B48" s="1"/>
+        <stp>zc1yRate</stp>
+        <stp>0</stp>
+        <tr r="B12" s="1"/>
       </tp>
+      <tp t="s">
+        <v>s2yratehelpers</v>
+        <stp/>
+        <stp>s2yratehelpers</stp>
+        <stp>-63164760</stp>
+        <tr r="K28" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
         <v>couponRate2</v>
         <stp/>
@@ -1295,132 +1488,326 @@
         <tr r="J16" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>libor3mPeriod</v>
+        <v>bondhelper2</v>
         <stp/>
-        <stp>libor3mPeriod</stp>
-        <stp>-1226026113</stp>
-        <tr r="B40" s="1"/>
+        <stp>bondhelper2</stp>
+        <stp>-1677774977</stp>
+        <tr r="M16" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>4.4999999999999998E-2</v>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>d9m</v>
         <stp/>
-        <stp>FixedZeroPreviouscoupon</stp>
-        <stp/>
-        <tr r="C68" s="1"/>
+        <stp>d9m</stp>
+        <stp>-1226026273</stp>
+        <tr r="H26" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>settlementDays</v>
+        <v>bondhelper0</v>
         <stp/>
-        <stp>settlementDays</stp>
-        <stp>3</stp>
-        <tr r="B6" s="1"/>
+        <stp>bondhelper0</stp>
+        <stp>1862217599</stp>
+        <tr r="M14" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>depoSwapTermStructure</v>
-        <stp/>
-        <stp>depoSwapTermStructure</stp>
-        <stp>-1492299688</stp>
-        <tr r="B19" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>discount</v>
-        <stp/>
-        <stp>discount</stp>
-        <stp>0</stp>
-        <tr r="E42" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>calendar</v>
-        <stp/>
-        <stp>calendar</stp>
-        <stp>0</stp>
-        <tr r="B2" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>bondhelper4</v>
-        <stp/>
-        <stp>bondhelper4</stp>
-        <stp>-1090572417</stp>
-        <tr r="M18" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>couponRate4</v>
-        <stp/>
-        <stp>couponRate4</stp>
-        <stp>1325718839</stp>
-        <tr r="J18" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
       <tp>
-        <v>86.317292342665496</v>
-        <stp/>
-        <stp>ZeroCleanPrice</stp>
-        <stp/>
-        <tr r="B65" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>2.8862499999999999E-2</v>
+        <v>3.4298412186850417E-2</v>
         <stp/>
         <stp>FloatingFixedZeroPreviouscoupon</stp>
         <stp/>
         <tr r="D68" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>schedule2</v>
+        <v>d1m</v>
         <stp/>
-        <stp>schedule2</stp>
-        <stp>1913417000</stp>
-        <tr r="L16" s="1"/>
+        <stp>d1m</stp>
+        <stp>-1226026145</stp>
+        <tr r="H23" s="1"/>
       </tp>
       <tp t="s">
-        <v>schedule3</v>
+        <v>d3m</v>
         <stp/>
-        <stp>schedule3</stp>
-        <stp>1913417000</stp>
-        <tr r="L17" s="1"/>
+        <stp>d3m</stp>
+        <stp>-1226026113</stp>
+        <tr r="H24" s="1"/>
       </tp>
       <tp t="s">
-        <v>schedule0</v>
+        <v>d6m</v>
         <stp/>
-        <stp>schedule0</stp>
-        <stp>1913417000</stp>
-        <tr r="L14" s="1"/>
+        <stp>d6m</stp>
+        <stp>-1226026161</stp>
+        <tr r="H25" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>depoSwapInstruments</v>
+        <stp/>
+        <stp>depoSwapInstruments</stp>
+        <stp>-501517731</stp>
+        <tr r="B18" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>couponRate1</v>
+        <stp/>
+        <stp>couponRate1</stp>
+        <stp>1162275258</stp>
+        <tr r="J15" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>zc3m</v>
+        <stp/>
+        <stp>zc3m</stp>
+        <stp>-1010340904</stp>
+        <tr r="H8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>bondDiscountingTermStructure</v>
+        <stp/>
+        <stp>bondDiscountingTermStructure</stp>
+        <stp>-1358081960</stp>
+        <tr r="B17" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>Semiannual</v>
+        <stp/>
+        <stp>Semiannual</stp>
+        <stp>1704154923</stp>
+        <tr r="E39" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>0.60974954998845188</v>
+        <stp/>
+        <stp>FloatingFixedZeroAccruedcoupon</stp>
+        <stp/>
+        <tr r="D67" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>marketQuotes4</v>
+        <stp/>
+        <stp>marketQuotes4</stp>
+        <stp>0</stp>
+        <tr r="K18" s="1"/>
       </tp>
       <tp t="s">
-        <v>schedule1</v>
+        <v>FixedSettlementDatte</v>
         <stp/>
-        <stp>schedule1</stp>
-        <stp>1913417000</stp>
-        <tr r="L15" s="1"/>
+        <stp>FixedSettlementDatte</stp>
+        <stp>-798541351</stp>
+        <tr r="B33" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>couponRate0</v>
+        <stp/>
+        <stp>couponRate0</stp>
+        <stp>-1165563463</stp>
+        <tr r="J14" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>marketQuotes3</v>
+        <stp/>
+        <stp>marketQuotes3</stp>
+        <stp>0</stp>
+        <tr r="K17" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>marketQuotes2</v>
+        <stp/>
+        <stp>marketQuotes2</stp>
+        <stp>0</stp>
+        <tr r="K16" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>swFloatingLegIndex</v>
+        <stp/>
+        <stp>swFloatingLegIndex</stp>
+        <stp>0</stp>
+        <tr r="E46" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>86.317292342665496</v>
+        <stp/>
+        <stp>ZeroDirtyPrice</stp>
+        <stp/>
+        <tr r="B66" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>marketQuotes1</v>
+        <stp/>
+        <stp>marketQuotes1</stp>
+        <stp>0</stp>
+        <tr r="K15" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>d1w</v>
+        <stp/>
+        <stp>d1w</stp>
+        <stp>-303078293</stp>
+        <tr r="H22" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>marketQuotes0</v>
+        <stp/>
+        <stp>marketQuotes0</stp>
+        <stp>0</stp>
+        <tr r="K14" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FixedZeroPreviouscoupon</v>
+        <stp/>
+        <stp>FixedZeroPreviouscoupon</stp>
+        <stp>815396861</stp>
+        <tr r="C60" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>s2y</v>
+        <stp/>
+        <stp>s2y</stp>
+        <stp>2119925512</stp>
+        <tr r="H28" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>zc1y</v>
+        <stp/>
+        <stp>zc1y</stp>
+        <stp>-2050528296</stp>
+        <tr r="H10" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>s3y</v>
+        <stp/>
+        <stp>s3y</stp>
+        <stp>2119925496</stp>
+        <tr r="H29" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>s5y</v>
+        <stp/>
+        <stp>s5y</stp>
+        <stp>2119925400</stp>
+        <tr r="H30" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>d1y</v>
+        <stp/>
+        <stp>d1y</stp>
+        <stp>2119925464</stp>
+        <tr r="H27" s="1"/>
       </tp>
       <tp t="s">
-        <v>schedule4</v>
+        <v>floatcouponpricer2</v>
         <stp/>
-        <stp>schedule4</stp>
-        <stp>1913417000</stp>
-        <tr r="L18" s="1"/>
+        <stp>floatcouponpricer2</stp>
+        <stp>1878722209</stp>
+        <tr r="B51" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>+settlementDateAdjustedSer</v>
+        <stp/>
+        <stp>+settlementDateAdjustedSer</stp>
+        <stp>-649169906</stp>
+        <tr r="C4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>faceAmount</v>
+        <stp/>
+        <stp>faceAmount</stp>
+        <stp>1079574528</stp>
+        <tr r="B24" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FixedRateCashflow</v>
+        <stp/>
+        <stp>FixedRateCashflow</stp>
+        <stp>-77321281</stp>
+        <tr r="B38" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>d3mRate</v>
+        <stp/>
+        <stp>d3mRate</stp>
+        <stp>0</stp>
+        <tr r="J24" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d1mRate</v>
+        <stp/>
+        <stp>d1mRate</stp>
+        <stp>0</stp>
+        <tr r="J23" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d6mRate</v>
+        <stp/>
+        <stp>d6mRate</stp>
+        <stp>0</stp>
+        <tr r="J25" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>d9mRate</v>
+        <stp/>
+        <stp>d9mRate</stp>
+        <stp>0</stp>
+        <tr r="J26" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
         <v>zc3mRate</v>
         <stp/>
@@ -1435,208 +1822,107 @@
         <stp>0</stp>
         <tr r="B11" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>Quarterly</v>
+        <v>bondhelper3</v>
         <stp/>
-        <stp>Quarterly</stp>
-        <stp>-302169631</stp>
-        <tr r="E49" s="1"/>
+        <stp>bondhelper3</stp>
+        <stp>922693503</stp>
+        <tr r="M17" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>3.0000642156600955E-2</v>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FixedNPV</v>
         <stp/>
-        <stp>ZeroYield</stp>
-        <stp/>
-        <tr r="B70" s="1"/>
+        <stp>FixedNPV</stp>
+        <stp>-77321281</stp>
+        <tr r="C56" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>s2y</v>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>1.5407608695652275</v>
         <stp/>
-        <stp>s2y</stp>
-        <stp>2119925512</stp>
-        <tr r="H28" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>FixedRateCashflow</v>
+        <stp>FixedZeroAccruedcoupon</stp>
         <stp/>
-        <stp>FixedRateCashflow</stp>
-        <stp>-77321281</stp>
-        <tr r="B38" s="1"/>
+        <tr r="C67" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>s5y</v>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>4.4999999999999998E-2</v>
         <stp/>
-        <stp>s5y</stp>
-        <stp>2119925400</stp>
-        <tr r="H30" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>s3y</v>
+        <stp>FixedNextcoupon</stp>
         <stp/>
-        <stp>s3y</stp>
-        <stp>2119925496</stp>
-        <tr r="H29" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d1y</v>
-        <stp/>
-        <stp>d1y</stp>
-        <stp>2119925464</stp>
-        <tr r="H27" s="1"/>
+        <tr r="C69" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FixedSettlementDatte</v>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>39706</v>
         <stp/>
-        <stp>FixedSettlementDatte</stp>
-        <stp>-798541351</stp>
-        <tr r="B33" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>marketQuotes4</v>
+        <stp>todaysDateSer</stp>
         <stp/>
-        <stp>marketQuotes4</stp>
-        <stp>0</stp>
-        <tr r="K18" s="1"/>
+        <tr r="D8" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>s10yratehelpers</v>
+        <v>fixingDaysNeg</v>
         <stp/>
-        <stp>s10yratehelpers</stp>
-        <stp>154939048</stp>
-        <tr r="K31" s="1"/>
+        <stp>fixingDaysNeg</stp>
+        <stp>-3</stp>
+        <tr r="B7" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FloatingNPV</v>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>2.2009365270878184E-2</v>
         <stp/>
-        <stp>FloatingNPV</stp>
-        <stp>588410313</stp>
-        <tr r="D56" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>todaysDateSer</v>
+        <stp>FloatingYield</stp>
         <stp/>
-        <stp>todaysDateSer</stp>
-        <stp>-1204259704</stp>
-        <tr r="C8" s="1"/>
+        <tr r="D70" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>d1w</v>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>106.127528263039</v>
         <stp/>
-        <stp>d1w</stp>
-        <stp>-303078293</stp>
-        <tr r="H22" s="1"/>
+        <stp>FixedCleanPrice</stp>
+        <stp/>
+        <tr r="C65" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>0.56211286639560409</v>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FloatingNextcoupon</v>
         <stp/>
-        <stp>FloatingFixedZeroAccruedcoupon</stp>
-        <stp/>
-        <tr r="D67" s="1"/>
+        <stp>FloatingNextcoupon</stp>
+        <stp>-1208119139</stp>
+        <tr r="D61" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>marketQuotes0</v>
+        <v>fixingDays</v>
         <stp/>
-        <stp>marketQuotes0</stp>
-        <stp>0</stp>
-        <tr r="K14" s="1"/>
+        <stp>fixingDays</stp>
+        <stp>3</stp>
+        <tr r="B5" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>marketQuotes1</v>
+        <v>FixedRateBond</v>
         <stp/>
-        <stp>marketQuotes1</stp>
-        <stp>0</stp>
-        <tr r="K15" s="1"/>
+        <stp>FixedRateBond</stp>
+        <stp>1820916808</stp>
+        <tr r="B37" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>marketQuotes2</v>
-        <stp/>
-        <stp>marketQuotes2</stp>
-        <stp>0</stp>
-        <tr r="K16" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ZeroAccruedcoupon</v>
-        <stp/>
-        <stp>ZeroAccruedcoupon</stp>
-        <stp>1029105693</stp>
-        <tr r="B59" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>86.317292342665496</v>
-        <stp/>
-        <stp>ZeroDirtyPrice</stp>
-        <stp/>
-        <tr r="B66" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>couponRate0</v>
-        <stp/>
-        <stp>couponRate0</stp>
-        <stp>-1165563463</stp>
-        <tr r="J14" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>marketQuotes3</v>
-        <stp/>
-        <stp>marketQuotes3</stp>
-        <stp>0</stp>
-        <tr r="K17" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>0</v>
-        <stp/>
-        <stp>ZeroAccruedcoupon</stp>
-        <stp/>
-        <tr r="B67" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>s15yratehelpers</v>
-        <stp/>
-        <stp>s15yratehelpers</stp>
-        <stp>-96719192</stp>
-        <tr r="K32" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>Actual365Fixed</v>
-        <stp/>
-        <stp>Actual365Fixed</stp>
-        <stp>0</stp>
-        <tr r="E50" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
         <v>USDLibor</v>
         <stp/>
@@ -1645,210 +1931,161 @@
         <tr r="J37" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>FixedRateBondzeroCouponBondCashflow</v>
+        <v>ZeroYield</v>
         <stp/>
-        <stp>FixedRateBondzeroCouponBondCashflow</stp>
-        <stp>CT</stp>
-        <tr r="H45" s="1"/>
-        <tr r="H48" s="1"/>
-        <tr r="I51" s="1"/>
-        <tr r="I54" s="1"/>
-        <tr r="I63" s="1"/>
-        <tr r="I52" s="1"/>
-        <tr r="I42" s="1"/>
-        <tr r="H58" s="1"/>
-        <tr r="H51" s="1"/>
-        <tr r="H55" s="1"/>
-        <tr r="I46" s="1"/>
-        <tr r="H46" s="1"/>
-        <tr r="I56" s="1"/>
-        <tr r="H56" s="1"/>
-        <tr r="I59" s="1"/>
-        <tr r="H49" s="1"/>
-        <tr r="I55" s="1"/>
-        <tr r="I45" s="1"/>
-        <tr r="H42" s="1"/>
-        <tr r="H50" s="1"/>
-        <tr r="I60" s="1"/>
-        <tr r="H61" s="1"/>
-        <tr r="I44" s="1"/>
-        <tr r="H43" s="1"/>
-        <tr r="I62" s="1"/>
-        <tr r="H53" s="1"/>
-        <tr r="H63" s="1"/>
-        <tr r="H54" s="1"/>
-        <tr r="H44" s="1"/>
-        <tr r="H52" s="1"/>
-        <tr r="H47" s="1"/>
-        <tr r="I58" s="1"/>
-        <tr r="I50" s="1"/>
-        <tr r="I57" s="1"/>
-        <tr r="I53" s="1"/>
-        <tr r="H57" s="1"/>
-        <tr r="H59" s="1"/>
-        <tr r="H60" s="1"/>
-        <tr r="I47" s="1"/>
-        <tr r="I61" s="1"/>
-        <tr r="H62" s="1"/>
-        <tr r="I48" s="1"/>
-        <tr r="I49" s="1"/>
-        <tr r="I43" s="1"/>
+        <stp>ZeroYield</stp>
+        <stp>-1391670259</stp>
+        <tr r="B62" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>optionletvolitility</v>
+        <v>depositDayCounter</v>
         <stp/>
-        <stp>optionletvolitility</stp>
-        <stp>0</stp>
-        <tr r="B49" s="1"/>
+        <stp>depositDayCounter</stp>
+        <stp>372029375</stp>
+        <tr r="E43" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>s10y</v>
+        <stp/>
+        <stp>s10y</stp>
+        <stp>1121190872</stp>
+        <tr r="H31" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>ConstantOptionletVolatility</v>
+        <v>zcBondsDayCounter</v>
         <stp/>
-        <stp>ConstantOptionletVolatility</stp>
-        <stp>315382730</stp>
-        <tr r="B50" s="1"/>
+        <stp>zcBondsDayCounter</stp>
+        <stp>0</stp>
+        <tr r="B9" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>s5yratehelpers</v>
+        <v>FloatingYield</v>
         <stp/>
-        <stp>s5yratehelpers</stp>
-        <stp>1362898600</stp>
-        <tr r="K30" s="1"/>
+        <stp>FloatingYield</stp>
+        <stp>-712193011</stp>
+        <tr r="D62" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>FixedCleanPrice</v>
+        <stp/>
+        <stp>FixedCleanPrice</stp>
+        <stp>-77321281</stp>
+        <tr r="C57" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>s3yratehelpers</v>
+        <v>forwardStart</v>
         <stp/>
-        <stp>s3yratehelpers</stp>
-        <stp>-751030616</stp>
-        <tr r="K29" s="1"/>
+        <stp>forwardStart</stp>
+        <stp>-223693829</stp>
+        <tr r="E47" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>FloatingNextcoupon</v>
+        <v>zc6m</v>
         <stp/>
-        <stp>FloatingNextcoupon</stp>
-        <stp>-1208119139</stp>
-        <tr r="D61" s="1"/>
+        <stp>zc6m</stp>
+        <stp>-792237096</stp>
+        <tr r="H9" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>4.4999999999999998E-2</v>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>tolerance</v>
         <stp/>
-        <stp>FixedNextcoupon</stp>
-        <stp/>
-        <tr r="C69" s="1"/>
+        <stp>tolerance</stp>
+        <stp>-1573562951</stp>
+        <tr r="B14" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>1.5407608695652275</v>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>todaysDate</v>
         <stp/>
-        <stp>FixedZeroAccruedcoupon</stp>
-        <stp/>
-        <tr r="C67" s="1"/>
+        <stp>todaysDate</stp>
+        <stp>-111422835</stp>
+        <tr r="B8" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>ZeroCleanPrice</v>
+        <v>fixedBondSchedule</v>
         <stp/>
-        <stp>ZeroCleanPrice</stp>
-        <stp>1001970241</stp>
-        <tr r="B57" s="1"/>
+        <stp>fixedBondSchedule</stp>
+        <stp>-2089128530</stp>
+        <tr r="B35" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>loglinier</v>
+        <stp/>
+        <stp>loglinier</stp>
+        <stp>0</stp>
+        <tr r="E44" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FixedDirtyPrice</v>
+        <stp/>
+        <stp>FixedDirtyPrice</stp>
+        <stp>-77321281</stp>
+        <tr r="C58" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>86.317292342665496</v>
+        <stp/>
+        <stp>ZeroNPV</stp>
+        <stp/>
+        <tr r="B64" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
+      <tp>
+        <v>107.66828913260423</v>
+        <stp/>
+        <stp>FixedDirtyPrice</stp>
+        <stp/>
+        <tr r="C66" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>FixedYield</v>
+        <stp/>
+        <stp>FixedYield</stp>
+        <stp>-1293104115</stp>
+        <tr r="C62" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
+      <tp t="s">
+        <v>zc6mPeriod</v>
+        <stp/>
+        <stp>zc6mPeriod</stp>
+        <stp>-1226026161</stp>
+        <tr r="E9" s="1"/>
       </tp>
       <tp t="s">
-        <v>d1yratehelpers</v>
+        <v>zc3mPeriod</v>
         <stp/>
-        <stp>d1yratehelpers</stp>
-        <stp>-499372376</stp>
-        <tr r="K27" s="1"/>
+        <stp>zc3mPeriod</stp>
+        <stp>-1226026113</stp>
+        <tr r="E8" s="1"/>
       </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FixedRateBondzeroCouponBondCashflow</v>
-        <stp/>
-        <stp>FixedRateBondzeroCouponBondCashflow</stp>
-        <stp>-77321281</stp>
-        <tr r="C63" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FloatIssueDate</v>
-        <stp/>
-        <stp>FloatIssueDate</stp>
-        <stp>451725283</stp>
-        <tr r="B43" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>106.127528263039</v>
-        <stp/>
-        <stp>FixedCleanPrice</stp>
-        <stp/>
-        <tr r="C65" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>RemptionAmount</v>
-        <stp/>
-        <stp>RemptionAmount</stp>
-        <stp>1079574528</stp>
-        <tr r="B25" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>d1wratehelpers</v>
-        <stp/>
-        <stp>d1wratehelpers</stp>
-        <stp>1144794792</stp>
-        <tr r="K22" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FixedNPV</v>
-        <stp/>
-        <stp>FixedNPV</stp>
-        <stp>-77321281</stp>
-        <tr r="C56" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>zeroCouponBondCashflow</v>
-        <stp/>
-        <stp>zeroCouponBondCashflow</stp>
-        <stp>1001970241</stp>
-        <tr r="B63" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>FixedIssueDate</v>
-        <stp/>
-        <stp>FixedIssueDate</stp>
-        <stp>996172436</stp>
-        <tr r="B34" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
       <tp t="s">
         <v>swFixedLegDayCounter</v>
         <stp/>
@@ -1858,25 +2095,7 @@
         <tr r="E51" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>bondEnginez</v>
-        <stp/>
-        <stp>bondEnginez</stp>
-        <stp>246307230</stp>
-        <tr r="B20" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>ZeroSettlementDate</v>
-        <stp/>
-        <stp>ZeroSettlementDate</stp>
-        <stp>-1699218839</stp>
-        <tr r="B27" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+    <main first="rtdsrv.bd21e641ad4a453fb7ffb814610b8360">
       <tp>
         <v>39709</v>
         <stp/>
@@ -1885,217 +2104,13 @@
         <tr r="D4" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
+    <main first="rtdsrv.bd714e49b28c452ebccede730ffe499a">
       <tp t="s">
-        <v>floatingRateBondFixedRateBondzeroCouponBondCashflow</v>
+        <v>ZeroSettlementDate</v>
         <stp/>
-        <stp>floatingRateBondFixedRateBondzeroCouponBondCashflow</stp>
-        <stp>CT</stp>
-        <tr r="I70" s="1"/>
-        <tr r="I72" s="1"/>
-        <tr r="H72" s="1"/>
-        <tr r="H66" s="1"/>
-        <tr r="H69" s="1"/>
-        <tr r="H83" s="1"/>
-        <tr r="I65" s="1"/>
-        <tr r="H84" s="1"/>
-        <tr r="I82" s="1"/>
-        <tr r="I81" s="1"/>
-        <tr r="H85" s="1"/>
-        <tr r="H65" s="1"/>
-        <tr r="H76" s="1"/>
-        <tr r="H75" s="1"/>
-        <tr r="H68" s="1"/>
-        <tr r="I80" s="1"/>
-        <tr r="H80" s="1"/>
-        <tr r="H73" s="1"/>
-        <tr r="H71" s="1"/>
-        <tr r="H77" s="1"/>
-        <tr r="I83" s="1"/>
-        <tr r="I77" s="1"/>
-        <tr r="H67" s="1"/>
-        <tr r="I74" s="1"/>
-        <tr r="I84" s="1"/>
-        <tr r="I85" s="1"/>
-        <tr r="I75" s="1"/>
-        <tr r="I73" s="1"/>
-        <tr r="I66" s="1"/>
-        <tr r="I67" s="1"/>
-        <tr r="H74" s="1"/>
-        <tr r="H79" s="1"/>
-        <tr r="I79" s="1"/>
-        <tr r="I64" s="1"/>
-        <tr r="I78" s="1"/>
-        <tr r="H82" s="1"/>
-        <tr r="H78" s="1"/>
-        <tr r="I68" s="1"/>
-        <tr r="H81" s="1"/>
-        <tr r="I71" s="1"/>
-        <tr r="H70" s="1"/>
-        <tr r="H64" s="1"/>
-        <tr r="I69" s="1"/>
-        <tr r="I76" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>USgovi</v>
-        <stp/>
-        <stp>USgovi</stp>
-        <stp>814714544</stp>
-        <tr r="E38" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>FixedYield</v>
-        <stp/>
-        <stp>FixedYield</stp>
-        <stp>-1293104115</stp>
-        <tr r="C62" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d3mratehelpers</v>
-        <stp/>
-        <stp>d3mratehelpers</stp>
-        <stp>1144794792</stp>
-        <tr r="K24" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>USDLibor1</v>
-        <stp/>
-        <stp>USDLibor1</stp>
-        <stp>2003614270</stp>
-        <tr r="J39" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>zc6mPeriod</v>
-        <stp/>
-        <stp>zc6mPeriod</stp>
-        <stp>-1226026161</stp>
-        <tr r="E9" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>zc3mPeriod</v>
-        <stp/>
-        <stp>zc3mPeriod</stp>
-        <stp>-1226026113</stp>
-        <tr r="E8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>zc6m</v>
-        <stp/>
-        <stp>zc6m</stp>
-        <stp>-792237096</stp>
-        <tr r="H9" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>d9mratehelpers</v>
-        <stp/>
-        <stp>d9mratehelpers</stp>
-        <stp>-969134424</stp>
-        <tr r="K26" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>forwardStart</v>
-        <stp/>
-        <stp>forwardStart</stp>
-        <stp>-223693829</stp>
-        <tr r="E47" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>zcBondsDayCounter</v>
-        <stp/>
-        <stp>zcBondsDayCounter</stp>
-        <stp>0</stp>
-        <tr r="B9" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>86.317292342665496</v>
-        <stp/>
-        <stp>ZeroNPV</stp>
-        <stp/>
-        <tr r="B64" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>d6mratehelpers</v>
-        <stp/>
-        <stp>d6mratehelpers</stp>
-        <stp>-449040728</stp>
-        <tr r="K25" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>s10y</v>
-        <stp/>
-        <stp>s10y</stp>
-        <stp>1121190872</stp>
-        <tr r="H31" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>depositDayCounter</v>
-        <stp/>
-        <stp>depositDayCounter</stp>
-        <stp>372029375</stp>
-        <tr r="E43" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>107.66828913260423</v>
-        <stp/>
-        <stp>FixedDirtyPrice</stp>
-        <stp/>
-        <tr r="C66" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>loglinier</v>
-        <stp/>
-        <stp>loglinier</stp>
-        <stp>0</stp>
-        <tr r="E44" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.aa0dc8c721934bdc8ed25b6f816d1c25">
-      <tp>
-        <v>107.66828913260423</v>
-        <stp/>
-        <stp>FixedNPV</stp>
-        <stp/>
-        <tr r="C64" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>ZeroDirtyPrice</v>
-        <stp/>
-        <stp>ZeroDirtyPrice</stp>
-        <stp>1001970241</stp>
-        <tr r="B58" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.32e84632adf54530927886b6879595f3">
-      <tp t="s">
-        <v>floatingRateBondFixedRateBondzeroCouponBondCashflow</v>
-        <stp/>
-        <stp>floatingRateBondFixedRateBondzeroCouponBondCashflow</stp>
-        <stp>588410313</stp>
-        <tr r="D63" s="1"/>
+        <stp>ZeroSettlementDate</stp>
+        <stp>-1699218839</stp>
+        <tr r="B27" s="1"/>
       </tp>
     </main>
   </volType>
@@ -2437,8 +2452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28025E14-2DBA-4FA2-A060-A0CB22BD8F4F}">
   <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3885,7 +3900,7 @@
       </c>
       <c r="B61" t="str">
         <f>+_xll._Bond_nextCouponRate(B$55&amp;$A61,B54)</f>
-        <v>ZeroNextcoupon</v>
+        <v>#no coupon paid at cashflow date 15/08/2013</v>
       </c>
       <c r="C61" t="str">
         <f>+_xll._Bond_nextCouponRate(C$55&amp;$A61,C54)</f>
@@ -4039,7 +4054,7 @@
       </c>
       <c r="D67">
         <f>+_xll._Value(D59)</f>
-        <v>0.56211286639560409</v>
+        <v>0.60974954998845188</v>
       </c>
       <c r="H67" t="str">
         <v>#NA</v>
@@ -4063,7 +4078,7 @@
       </c>
       <c r="D68">
         <f>+_xll._Value(D60)</f>
-        <v>2.8862499999999999E-2</v>
+        <v>3.4298412186850417E-2</v>
       </c>
       <c r="H68" t="str">
         <v>#NA</v>
@@ -4079,7 +4094,7 @@
       </c>
       <c r="B69" t="str">
         <f>+_xll._Value(B61)</f>
-        <v>#no coupon paid at cashflow date 15/08/2013 ,Bond.nextCouponRate</v>
+        <v>#NA</v>
       </c>
       <c r="C69">
         <f>+_xll._Value(C61)</f>
@@ -4103,7 +4118,7 @@
       </c>
       <c r="B70">
         <f>+_xll._Value(B62)</f>
-        <v>3.0000642156600955E-2</v>
+        <v>3.0058566999435425E-2</v>
       </c>
       <c r="C70">
         <f>+_xll._Value(C62)</f>

</xml_diff>